<commit_message>
Escaleta columna F izquierda
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/ESCALETA_CN_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/ESCALETA_CN_08_04_CO.xlsx
@@ -12,9 +12,6 @@
     <sheet name="VER" sheetId="3" r:id="rId3"/>
     <sheet name="Recursos alterados" sheetId="4" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -884,7 +881,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -965,21 +962,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -1175,12 +1157,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1224,14 +1232,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1240,7 +1248,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1251,19 +1259,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1280,64 +1288,67 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1356,23 +1367,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ESCALETA"/>
-      <sheetName val="DATOS"/>
-      <sheetName val="VER"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1630,7 +1624,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1640,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,8 +1651,8 @@
     <col min="10" max="10" width="92.28515625" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" style="4" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="14" style="4" customWidth="1"/>
     <col min="15" max="15" width="60" style="5" customWidth="1"/>
     <col min="16" max="16" width="16.42578125" style="2" customWidth="1"/>
     <col min="17" max="17" width="10.42578125" customWidth="1"/>
@@ -1669,94 +1663,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="65" t="s">
+      <c r="G1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="74" t="s">
+      <c r="K1" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="69" t="s">
+      <c r="L1" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="73" t="s">
+      <c r="M1" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="73"/>
-      <c r="O1" s="67" t="s">
+      <c r="N1" s="79"/>
+      <c r="O1" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="69" t="s">
+      <c r="P1" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="65" t="s">
+      <c r="Q1" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="69" t="s">
+      <c r="R1" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="71" t="s">
+      <c r="S1" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="69" t="s">
+      <c r="T1" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="71" t="s">
+      <c r="U1" s="65" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="7" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="66"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="70"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="68"/>
       <c r="M2" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="N2" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="O2" s="68"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="72"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="68"/>
+      <c r="U2" s="66"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -1793,10 +1787,10 @@
       <c r="L3" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="31"/>
-      <c r="N3" s="32" t="s">
+      <c r="M3" s="32" t="s">
         <v>36</v>
       </c>
+      <c r="N3" s="31"/>
       <c r="O3" s="45" t="s">
         <v>185</v>
       </c>
@@ -1854,10 +1848,10 @@
       <c r="L4" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="31" t="s">
+      <c r="M4" s="32"/>
+      <c r="N4" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="N4" s="32"/>
       <c r="O4" s="45" t="s">
         <v>197</v>
       </c>
@@ -1915,10 +1909,10 @@
       <c r="L5" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="32"/>
+      <c r="N5" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="N5" s="32"/>
       <c r="O5" s="45" t="s">
         <v>194</v>
       </c>
@@ -1976,10 +1970,10 @@
       <c r="L6" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="31" t="s">
+      <c r="M6" s="32"/>
+      <c r="N6" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="N6" s="32"/>
       <c r="O6" s="45"/>
       <c r="P6" s="54" t="s">
         <v>19</v>
@@ -2033,10 +2027,10 @@
       <c r="L7" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="31"/>
-      <c r="N7" s="32" t="s">
+      <c r="M7" s="32" t="s">
         <v>36</v>
       </c>
+      <c r="N7" s="31"/>
       <c r="O7" s="45" t="s">
         <v>199</v>
       </c>
@@ -2096,10 +2090,10 @@
       <c r="L8" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="31" t="s">
+      <c r="M8" s="32"/>
+      <c r="N8" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="N8" s="32"/>
       <c r="O8" s="45"/>
       <c r="P8" s="54" t="s">
         <v>19</v>
@@ -2157,10 +2151,10 @@
       <c r="L9" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="43" t="s">
+      <c r="M9" s="44"/>
+      <c r="N9" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="44"/>
       <c r="O9" s="45" t="s">
         <v>202</v>
       </c>
@@ -2220,10 +2214,10 @@
       <c r="L10" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="31" t="s">
+      <c r="M10" s="32"/>
+      <c r="N10" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="32"/>
       <c r="O10" s="45"/>
       <c r="P10" s="54" t="s">
         <v>19</v>
@@ -2279,10 +2273,10 @@
       <c r="L11" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="31" t="s">
+      <c r="M11" s="32"/>
+      <c r="N11" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="N11" s="32"/>
       <c r="O11" s="45" t="s">
         <v>232</v>
       </c>
@@ -2340,10 +2334,10 @@
       <c r="L12" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="31"/>
-      <c r="N12" s="32" t="s">
+      <c r="M12" s="32" t="s">
         <v>38</v>
       </c>
+      <c r="N12" s="31"/>
       <c r="O12" s="45" t="s">
         <v>204</v>
       </c>
@@ -2401,10 +2395,10 @@
       <c r="L13" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M13" s="31" t="s">
+      <c r="M13" s="32"/>
+      <c r="N13" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="N13" s="32"/>
       <c r="O13" s="45"/>
       <c r="P13" s="54" t="s">
         <v>19</v>
@@ -2460,10 +2454,10 @@
       <c r="L14" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M14" s="31" t="s">
+      <c r="M14" s="32"/>
+      <c r="N14" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="N14" s="32"/>
       <c r="O14" s="45" t="s">
         <v>235</v>
       </c>
@@ -2519,10 +2513,10 @@
       <c r="L15" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="M15" s="31"/>
-      <c r="N15" s="32" t="s">
+      <c r="M15" s="32" t="s">
         <v>39</v>
       </c>
+      <c r="N15" s="31"/>
       <c r="O15" s="45" t="s">
         <v>210</v>
       </c>
@@ -2578,8 +2572,8 @@
       <c r="L16" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="M16" s="31"/>
-      <c r="N16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="31"/>
       <c r="O16" s="45" t="s">
         <v>223</v>
       </c>
@@ -2635,10 +2629,10 @@
       <c r="L17" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="31" t="s">
+      <c r="M17" s="32"/>
+      <c r="N17" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="N17" s="32"/>
       <c r="O17" s="45"/>
       <c r="P17" s="54" t="s">
         <v>19</v>
@@ -2694,10 +2688,10 @@
       <c r="L18" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="31" t="s">
+      <c r="M18" s="32"/>
+      <c r="N18" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="N18" s="32"/>
       <c r="O18" s="45" t="s">
         <v>239</v>
       </c>
@@ -2753,10 +2747,10 @@
       <c r="L19" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="M19" s="31"/>
-      <c r="N19" s="32" t="s">
+      <c r="M19" s="32" t="s">
         <v>38</v>
       </c>
+      <c r="N19" s="31"/>
       <c r="O19" s="45" t="s">
         <v>214</v>
       </c>
@@ -2814,8 +2808,8 @@
       <c r="L20" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="31"/>
-      <c r="N20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="31"/>
       <c r="O20" s="45"/>
       <c r="P20" s="54" t="s">
         <v>19</v>
@@ -2873,10 +2867,10 @@
       <c r="L21" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M21" s="31" t="s">
+      <c r="M21" s="32"/>
+      <c r="N21" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="N21" s="32"/>
       <c r="O21" s="45"/>
       <c r="P21" s="54" t="s">
         <v>19</v>
@@ -2932,8 +2926,8 @@
       <c r="L22" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="M22" s="31"/>
-      <c r="N22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="31"/>
       <c r="O22" s="45" t="s">
         <v>223</v>
       </c>
@@ -2991,10 +2985,10 @@
       <c r="L23" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="31" t="s">
+      <c r="M23" s="32"/>
+      <c r="N23" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="N23" s="32"/>
       <c r="O23" s="45"/>
       <c r="P23" s="54" t="s">
         <v>19</v>
@@ -3050,10 +3044,10 @@
       <c r="L24" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="31" t="s">
+      <c r="M24" s="32"/>
+      <c r="N24" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="N24" s="32"/>
       <c r="O24" s="45"/>
       <c r="P24" s="54" t="s">
         <v>19</v>
@@ -3109,10 +3103,10 @@
       <c r="L25" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M25" s="31" t="s">
+      <c r="M25" s="32"/>
+      <c r="N25" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="N25" s="32"/>
       <c r="O25" s="45" t="s">
         <v>244</v>
       </c>
@@ -3170,10 +3164,10 @@
       <c r="L26" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="M26" s="31"/>
-      <c r="N26" s="32" t="s">
+      <c r="M26" s="32" t="s">
         <v>38</v>
       </c>
+      <c r="N26" s="31"/>
       <c r="O26" s="45"/>
       <c r="P26" s="54" t="s">
         <v>19</v>
@@ -3229,10 +3223,10 @@
       <c r="L27" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M27" s="31" t="s">
+      <c r="M27" s="32"/>
+      <c r="N27" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="N27" s="32"/>
       <c r="O27" s="45"/>
       <c r="P27" s="54" t="s">
         <v>19</v>
@@ -3288,10 +3282,10 @@
       <c r="L28" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M28" s="31" t="s">
+      <c r="M28" s="32"/>
+      <c r="N28" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="N28" s="32"/>
       <c r="O28" s="45"/>
       <c r="P28" s="54" t="s">
         <v>20</v>
@@ -3347,10 +3341,10 @@
       <c r="L29" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M29" s="31" t="s">
+      <c r="M29" s="32"/>
+      <c r="N29" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="N29" s="32"/>
       <c r="O29" s="45"/>
       <c r="P29" s="54" t="s">
         <v>19</v>
@@ -3404,10 +3398,10 @@
       <c r="L30" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M30" s="31" t="s">
+      <c r="M30" s="32"/>
+      <c r="N30" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="N30" s="32"/>
       <c r="O30" s="45"/>
       <c r="P30" s="54" t="s">
         <v>19</v>
@@ -3461,10 +3455,10 @@
       <c r="L31" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M31" s="31" t="s">
+      <c r="M31" s="32"/>
+      <c r="N31" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="N31" s="32"/>
       <c r="O31" s="45"/>
       <c r="P31" s="54" t="s">
         <v>19</v>
@@ -3518,8 +3512,8 @@
       <c r="L32" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="M32" s="31"/>
-      <c r="N32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="31"/>
       <c r="O32" s="45"/>
       <c r="P32" s="54" t="s">
         <v>19</v>
@@ -3563,10 +3557,10 @@
       <c r="L33" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M33" s="31" t="s">
+      <c r="M33" s="32"/>
+      <c r="N33" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="N33" s="32"/>
       <c r="O33" s="45"/>
       <c r="P33" s="54" t="s">
         <v>19</v>
@@ -3620,10 +3614,10 @@
       <c r="L34" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="M34" s="31" t="s">
+      <c r="M34" s="32"/>
+      <c r="N34" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="N34" s="32"/>
       <c r="O34" s="45"/>
       <c r="P34" s="54" t="s">
         <v>20</v>
@@ -3646,6 +3640,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3661,11 +3660,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3700,13 +3694,13 @@
           <x14:formula1>
             <xm:f>DATOS!$C$2:$C$39</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M34</xm:sqref>
+          <xm:sqref>N3:N34</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$2:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N34</xm:sqref>
+          <xm:sqref>M3:M34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4377,40 +4371,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="76" t="s">
+      <c r="G1" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="67" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="78"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="77"/>
     </row>
     <row r="3" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">

</xml_diff>

<commit_message>
Escaleta grupo 1 con anotaciones y mapa 09_05
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/ESCALETA_CN_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/ESCALETA_CN_08_04_CO.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="262">
   <si>
     <t>Asignatura</t>
   </si>
@@ -378,9 +378,6 @@
     <t>Identifica las partes de una flor</t>
   </si>
   <si>
-    <t>REC90</t>
-  </si>
-  <si>
     <t>Actividad para desarrollar destrezas en la identificación de las partes de una flor</t>
   </si>
   <si>
@@ -564,9 +561,6 @@
     <t>Los tipos de reproducción en la naturaleza</t>
   </si>
   <si>
-    <t>Recursos que cambian de lugar</t>
-  </si>
-  <si>
     <t>La reproducción vegetativa</t>
   </si>
   <si>
@@ -769,13 +763,58 @@
   </si>
   <si>
     <t>Actividad acerca de la reproducción de microorganismos</t>
+  </si>
+  <si>
+    <t>Recursos 1ra versión del guion</t>
+  </si>
+  <si>
+    <t>ORDEN</t>
+  </si>
+  <si>
+    <t>TITULO DE RECURSO</t>
+  </si>
+  <si>
+    <t>Reproducción y estrategias reproductivas</t>
+  </si>
+  <si>
+    <t>La reproducción asexual en los seres vivos</t>
+  </si>
+  <si>
+    <t>Selecciona cómo se reproducen estos organismos</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La reproducción en microorganismos</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Ventajas y desventajas de los tipos de reproducción</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La reproducción de los hongos</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La reproducción de las plantas</t>
+  </si>
+  <si>
+    <t>La función de reproducción</t>
+  </si>
+  <si>
+    <t>Competencias: análisis de crecimiento bacteriano</t>
+  </si>
+  <si>
+    <t>Nota: los nombres de estos recursos son los que se pusieron en la plataforma, algunos erróneamente. En algunos casos, al subirlos a la plataforma de dejaron los nombres originales de los recursos aprovechados, y no los nombres nuevos propuestos por el autor o el editor. Esto significa que estos nombres no coincidirán con lo que aparece en el guion que se usó para digitalizar este capítulo 08_04, pero sí son los recursos que actualmente están montados, y en el orden en el que están. No tengo acceso a los nombres que se propusieron en un principio.</t>
+  </si>
+  <si>
+    <t>Nota: los recursos en amarillo son recursos que aún no se han hecho, y no están en la plataforma</t>
+  </si>
+  <si>
+    <t>Los recursos en naranja son unos que ya están montados pero que requieren cambios importantes: el audio en los videos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -818,8 +857,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -880,6 +935,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -1188,7 +1273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1244,9 +1329,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1254,13 +1336,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1268,14 +1348,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1297,8 +1372,11 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1306,22 +1384,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1330,12 +1414,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1345,12 +1423,60 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1624,7 +1750,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1632,10 +1758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U34"/>
+  <dimension ref="A1:X37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:N1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,99 +1786,111 @@
     <col min="19" max="19" width="44.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="60.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" style="2"/>
+    <col min="24" max="24" width="80.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="78" t="s">
+      <c r="M1" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="79"/>
-      <c r="O1" s="69" t="s">
+      <c r="N1" s="67"/>
+      <c r="O1" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="63" t="s">
+      <c r="Q1" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="67" t="s">
+      <c r="R1" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="65" t="s">
+      <c r="S1" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="67" t="s">
+      <c r="T1" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="65" t="s">
+      <c r="U1" s="64" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" s="7" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="68"/>
+      <c r="W1" s="73" t="s">
+        <v>247</v>
+      </c>
+      <c r="X1" s="73"/>
+    </row>
+    <row r="2" spans="1:24" s="7" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="59"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="63"/>
       <c r="M2" s="23" t="s">
         <v>87</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="70"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="66"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="61"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="65"/>
+      <c r="W2" s="74" t="s">
+        <v>248</v>
+      </c>
+      <c r="X2" s="75" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>67</v>
       </c>
@@ -1766,54 +1904,60 @@
         <v>92</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F3" s="26"/>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="79">
         <v>1</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="J3" s="40" t="s">
-        <v>190</v>
+      <c r="J3" s="81" t="s">
+        <v>188</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="30" t="s">
+      <c r="L3" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="31"/>
-      <c r="O3" s="45" t="s">
+      <c r="N3" s="30"/>
+      <c r="O3" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="P3" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="51">
+        <v>6</v>
+      </c>
+      <c r="R3" s="49" t="s">
+        <v>184</v>
+      </c>
+      <c r="S3" s="49" t="s">
         <v>185</v>
       </c>
-      <c r="P3" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="57">
-        <v>6</v>
-      </c>
-      <c r="R3" s="55" t="s">
+      <c r="T3" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="S3" s="55" t="s">
+      <c r="U3" s="49" t="s">
         <v>187</v>
       </c>
-      <c r="T3" s="59" t="s">
-        <v>188</v>
-      </c>
-      <c r="U3" s="55" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W3" s="76">
+        <v>1</v>
+      </c>
+      <c r="X3" s="90" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>67</v>
       </c>
@@ -1827,54 +1971,60 @@
         <v>92</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F4" s="26"/>
-      <c r="G4" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="H4" s="13">
+      <c r="G4" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="H4" s="79">
         <v>2</v>
       </c>
-      <c r="I4" s="62" t="s">
+      <c r="I4" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="J4" s="40" t="s">
-        <v>191</v>
+      <c r="J4" s="81" t="s">
+        <v>189</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="32"/>
-      <c r="N4" s="31" t="s">
+      <c r="M4" s="31"/>
+      <c r="N4" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="45" t="s">
-        <v>197</v>
-      </c>
-      <c r="P4" s="54" t="s">
+      <c r="O4" s="42" t="s">
+        <v>195</v>
+      </c>
+      <c r="P4" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="58">
+      <c r="Q4" s="52">
         <v>6</v>
       </c>
-      <c r="R4" s="56" t="s">
+      <c r="R4" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="S4" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="S4" s="56" t="s">
-        <v>166</v>
-      </c>
-      <c r="T4" s="60" t="s">
-        <v>170</v>
-      </c>
-      <c r="U4" s="56" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T4" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="U4" s="50" t="s">
+        <v>167</v>
+      </c>
+      <c r="W4" s="76">
+        <v>2</v>
+      </c>
+      <c r="X4" s="90" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>67</v>
       </c>
@@ -1891,51 +2041,57 @@
         <v>95</v>
       </c>
       <c r="F5" s="26"/>
-      <c r="G5" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="H5" s="13">
+      <c r="G5" s="78" t="s">
+        <v>175</v>
+      </c>
+      <c r="H5" s="79">
         <v>3</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="J5" s="49" t="s">
-        <v>192</v>
+      <c r="J5" s="83" t="s">
+        <v>190</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="L5" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="32"/>
-      <c r="N5" s="31" t="s">
+      <c r="M5" s="31"/>
+      <c r="N5" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="45" t="s">
-        <v>194</v>
-      </c>
-      <c r="P5" s="54" t="s">
+      <c r="O5" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="P5" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="Q5" s="58">
+      <c r="Q5" s="52">
         <v>6</v>
       </c>
-      <c r="R5" s="56" t="s">
+      <c r="R5" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="S5" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="S5" s="56" t="s">
+      <c r="T5" s="54" t="s">
         <v>166</v>
       </c>
-      <c r="T5" s="60" t="s">
+      <c r="U5" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="U5" s="56" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W5" s="76">
+        <v>3</v>
+      </c>
+      <c r="X5" s="90" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>67</v>
       </c>
@@ -1953,7 +2109,7 @@
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H6" s="13">
         <v>4</v>
@@ -1961,40 +2117,46 @@
       <c r="I6" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="J6" s="40" t="s">
-        <v>193</v>
+      <c r="J6" s="37" t="s">
+        <v>191</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="30" t="s">
+      <c r="L6" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="32"/>
-      <c r="N6" s="31" t="s">
+      <c r="M6" s="31"/>
+      <c r="N6" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="O6" s="45"/>
-      <c r="P6" s="54" t="s">
+      <c r="O6" s="42"/>
+      <c r="P6" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="61">
+      <c r="Q6" s="55">
         <v>6</v>
       </c>
-      <c r="R6" s="52" t="s">
+      <c r="R6" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="S6" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="S6" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T6" s="53" t="s">
-        <v>195</v>
-      </c>
-      <c r="U6" s="52" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T6" s="47" t="s">
+        <v>193</v>
+      </c>
+      <c r="U6" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="W6" s="76">
+        <v>4</v>
+      </c>
+      <c r="X6" s="90" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>67</v>
       </c>
@@ -2009,51 +2171,57 @@
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="26"/>
-      <c r="G7" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="H7" s="13">
+      <c r="G7" s="78" t="s">
+        <v>178</v>
+      </c>
+      <c r="H7" s="79">
         <v>5</v>
       </c>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="J7" s="40" t="s">
-        <v>198</v>
+      <c r="J7" s="81" t="s">
+        <v>196</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="30" t="s">
+      <c r="L7" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="32" t="s">
+      <c r="M7" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="N7" s="31"/>
-      <c r="O7" s="45" t="s">
+      <c r="N7" s="30"/>
+      <c r="O7" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="P7" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="52">
+        <v>6</v>
+      </c>
+      <c r="R7" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="S7" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="T7" s="54" t="s">
         <v>199</v>
       </c>
-      <c r="P7" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q7" s="58">
-        <v>6</v>
-      </c>
-      <c r="R7" s="56" t="s">
-        <v>186</v>
-      </c>
-      <c r="S7" s="56" t="s">
+      <c r="U7" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="T7" s="60" t="s">
-        <v>201</v>
-      </c>
-      <c r="U7" s="56" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W7" s="76">
+        <v>5</v>
+      </c>
+      <c r="X7" s="90" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>67</v>
       </c>
@@ -2081,103 +2249,115 @@
       <c r="I8" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J8" s="40" t="s">
+      <c r="J8" s="37" t="s">
         <v>101</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="30" t="s">
+      <c r="L8" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="32"/>
-      <c r="N8" s="31" t="s">
+      <c r="M8" s="31"/>
+      <c r="N8" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="O8" s="45"/>
-      <c r="P8" s="54" t="s">
+      <c r="O8" s="42"/>
+      <c r="P8" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="58">
+      <c r="Q8" s="52">
         <v>6</v>
       </c>
-      <c r="R8" s="52" t="s">
+      <c r="R8" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="S8" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="S8" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T8" s="53" t="s">
-        <v>169</v>
-      </c>
-      <c r="U8" s="52" t="s">
+      <c r="T8" s="47" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="U8" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="W8" s="76">
+        <v>6</v>
+      </c>
+      <c r="X8" s="90" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" s="43" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="E9" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="F9" s="38" t="s">
-        <v>229</v>
-      </c>
-      <c r="G9" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="H9" s="13">
+      <c r="E9" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="G9" s="84" t="s">
+        <v>174</v>
+      </c>
+      <c r="H9" s="79">
         <v>7</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="J9" s="40" t="s">
+      <c r="J9" s="81" t="s">
+        <v>198</v>
+      </c>
+      <c r="K9" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="41"/>
+      <c r="N9" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="O9" s="42" t="s">
         <v>200</v>
       </c>
-      <c r="K9" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="L9" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9" s="44"/>
-      <c r="N9" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="O9" s="45" t="s">
-        <v>202</v>
-      </c>
-      <c r="P9" s="54" t="s">
+      <c r="P9" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="58">
+      <c r="Q9" s="52">
         <v>6</v>
       </c>
-      <c r="R9" s="52" t="s">
+      <c r="R9" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="S9" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="S9" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T9" s="53" t="s">
-        <v>233</v>
-      </c>
-      <c r="U9" s="52" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T9" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="U9" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="W9" s="76">
+        <v>7</v>
+      </c>
+      <c r="X9" s="90" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>67</v>
       </c>
@@ -2190,14 +2370,14 @@
       <c r="D10" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="F10" s="38" t="s">
-        <v>229</v>
+      <c r="E10" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>227</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H10" s="13">
         <v>8</v>
@@ -2205,40 +2385,46 @@
       <c r="I10" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J10" s="40" t="s">
+      <c r="J10" s="37" t="s">
         <v>108</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="30" t="s">
+      <c r="L10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="32"/>
-      <c r="N10" s="31" t="s">
+      <c r="M10" s="31"/>
+      <c r="N10" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="O10" s="45"/>
-      <c r="P10" s="54" t="s">
+      <c r="O10" s="42"/>
+      <c r="P10" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="58">
+      <c r="Q10" s="52">
         <v>6</v>
       </c>
-      <c r="R10" s="52" t="s">
+      <c r="R10" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="S10" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="S10" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T10" s="53" t="s">
-        <v>196</v>
-      </c>
-      <c r="U10" s="52" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T10" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="U10" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="W10" s="77">
+        <v>8</v>
+      </c>
+      <c r="X10" s="90" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>67</v>
       </c>
@@ -2251,55 +2437,61 @@
       <c r="D11" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="38"/>
-      <c r="G11" s="27" t="s">
-        <v>230</v>
-      </c>
-      <c r="H11" s="13">
+      <c r="F11" s="36"/>
+      <c r="G11" s="78" t="s">
+        <v>228</v>
+      </c>
+      <c r="H11" s="79">
         <v>9</v>
       </c>
-      <c r="I11" s="28" t="s">
+      <c r="I11" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="J11" s="40" t="s">
-        <v>231</v>
+      <c r="J11" s="81" t="s">
+        <v>229</v>
       </c>
       <c r="K11" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L11" s="30" t="s">
+      <c r="L11" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="32"/>
-      <c r="N11" s="31" t="s">
+      <c r="M11" s="31"/>
+      <c r="N11" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="O11" s="45" t="s">
-        <v>232</v>
-      </c>
-      <c r="P11" s="54" t="s">
+      <c r="O11" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="P11" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="58">
+      <c r="Q11" s="52">
         <v>6</v>
       </c>
-      <c r="R11" s="52" t="s">
+      <c r="R11" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="S11" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="S11" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T11" s="53" t="s">
-        <v>236</v>
-      </c>
-      <c r="U11" s="52" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T11" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="U11" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="W11" s="77">
+        <v>9</v>
+      </c>
+      <c r="X11" s="90" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>67</v>
       </c>
@@ -2313,54 +2505,60 @@
         <v>109</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F12" s="26"/>
-      <c r="G12" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="H12" s="13">
+      <c r="G12" s="78" t="s">
+        <v>182</v>
+      </c>
+      <c r="H12" s="79">
         <v>10</v>
       </c>
-      <c r="I12" s="28" t="s">
+      <c r="I12" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="J12" s="40" t="s">
-        <v>203</v>
+      <c r="J12" s="81" t="s">
+        <v>201</v>
       </c>
       <c r="K12" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="30" t="s">
+      <c r="L12" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="32" t="s">
+      <c r="M12" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="N12" s="31"/>
-      <c r="O12" s="45" t="s">
-        <v>204</v>
-      </c>
-      <c r="P12" s="54" t="s">
+      <c r="N12" s="30"/>
+      <c r="O12" s="42" t="s">
+        <v>202</v>
+      </c>
+      <c r="P12" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="58">
+      <c r="Q12" s="52">
         <v>6</v>
       </c>
-      <c r="R12" s="56" t="s">
-        <v>186</v>
-      </c>
-      <c r="S12" s="56" t="s">
+      <c r="R12" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="S12" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="T12" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="U12" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="T12" s="60" t="s">
-        <v>205</v>
-      </c>
-      <c r="U12" s="56" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W12" s="77">
+        <v>10</v>
+      </c>
+      <c r="X12" s="90" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>67</v>
       </c>
@@ -2374,11 +2572,11 @@
         <v>109</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="27" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H13" s="13">
         <v>11</v>
@@ -2386,40 +2584,46 @@
       <c r="I13" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J13" s="40" t="s">
-        <v>224</v>
+      <c r="J13" s="37" t="s">
+        <v>222</v>
       </c>
       <c r="K13" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="30" t="s">
+      <c r="L13" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M13" s="32"/>
-      <c r="N13" s="31" t="s">
+      <c r="M13" s="31"/>
+      <c r="N13" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="O13" s="45"/>
-      <c r="P13" s="54" t="s">
+      <c r="O13" s="42"/>
+      <c r="P13" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="58">
+      <c r="Q13" s="52">
         <v>6</v>
       </c>
-      <c r="R13" s="52" t="s">
+      <c r="R13" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="S13" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="S13" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T13" s="53" t="s">
-        <v>171</v>
-      </c>
-      <c r="U13" s="52" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T13" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="U13" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="W13" s="77">
+        <v>11</v>
+      </c>
+      <c r="X13" s="90" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>67</v>
       </c>
@@ -2436,51 +2640,57 @@
         <v>95</v>
       </c>
       <c r="F14" s="26"/>
-      <c r="G14" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="H14" s="13">
+      <c r="G14" s="78" t="s">
+        <v>205</v>
+      </c>
+      <c r="H14" s="79">
         <v>12</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="J14" s="40" t="s">
-        <v>248</v>
+      <c r="J14" s="81" t="s">
+        <v>246</v>
       </c>
       <c r="K14" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L14" s="30" t="s">
+      <c r="L14" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M14" s="32"/>
-      <c r="N14" s="31" t="s">
+      <c r="M14" s="31"/>
+      <c r="N14" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="O14" s="45" t="s">
+      <c r="O14" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="P14" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14" s="52">
+        <v>6</v>
+      </c>
+      <c r="R14" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="S14" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="T14" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="P14" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="58">
-        <v>6</v>
-      </c>
-      <c r="R14" s="52" t="s">
-        <v>165</v>
-      </c>
-      <c r="S14" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T14" s="53" t="s">
-        <v>237</v>
-      </c>
-      <c r="U14" s="52" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U14" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="W14" s="77">
+        <v>12</v>
+      </c>
+      <c r="X14" s="90" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>67</v>
       </c>
@@ -2495,51 +2705,57 @@
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="26"/>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="79">
         <v>13</v>
       </c>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="J15" s="40" t="s">
-        <v>209</v>
+      <c r="J15" s="81" t="s">
+        <v>207</v>
       </c>
       <c r="K15" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L15" s="30" t="s">
+      <c r="L15" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="M15" s="32" t="s">
+      <c r="M15" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="N15" s="31"/>
-      <c r="O15" s="45" t="s">
-        <v>210</v>
-      </c>
-      <c r="P15" s="54" t="s">
+      <c r="N15" s="30"/>
+      <c r="O15" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="P15" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="58">
+      <c r="Q15" s="52">
         <v>6</v>
       </c>
-      <c r="R15" s="56" t="s">
-        <v>186</v>
-      </c>
-      <c r="S15" s="56" t="s">
+      <c r="R15" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="S15" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="T15" s="54" t="s">
+        <v>209</v>
+      </c>
+      <c r="U15" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="T15" s="60" t="s">
-        <v>211</v>
-      </c>
-      <c r="U15" s="56" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W15" s="77">
+        <v>13</v>
+      </c>
+      <c r="X15" s="90" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>67</v>
       </c>
@@ -2554,49 +2770,55 @@
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="26"/>
-      <c r="G16" s="33" t="s">
-        <v>247</v>
-      </c>
-      <c r="H16" s="13">
+      <c r="G16" s="86" t="s">
+        <v>245</v>
+      </c>
+      <c r="H16" s="87">
         <v>14</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="88" t="s">
         <v>94</v>
       </c>
-      <c r="J16" s="40" t="s">
-        <v>212</v>
+      <c r="J16" s="89" t="s">
+        <v>210</v>
       </c>
       <c r="K16" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L16" s="30" t="s">
+      <c r="L16" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="M16" s="32"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="45" t="s">
-        <v>223</v>
-      </c>
-      <c r="P16" s="54" t="s">
+      <c r="M16" s="31"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="P16" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="58">
+      <c r="Q16" s="52">
         <v>6</v>
       </c>
-      <c r="R16" s="52" t="s">
+      <c r="R16" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="S16" s="52" t="s">
+      <c r="S16" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="T16" s="52" t="s">
+      <c r="T16" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="U16" s="52" t="s">
+      <c r="U16" s="46" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W16" s="77">
+        <v>14</v>
+      </c>
+      <c r="X16" s="90" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>67</v>
       </c>
@@ -2612,7 +2834,7 @@
       <c r="E17" s="12"/>
       <c r="F17" s="26"/>
       <c r="G17" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H17" s="13">
         <v>15</v>
@@ -2620,40 +2842,46 @@
       <c r="I17" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J17" s="40" t="s">
+      <c r="J17" s="37" t="s">
         <v>114</v>
       </c>
       <c r="K17" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L17" s="30" t="s">
+      <c r="L17" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="32"/>
-      <c r="N17" s="31" t="s">
+      <c r="M17" s="31"/>
+      <c r="N17" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="O17" s="45"/>
-      <c r="P17" s="54" t="s">
+      <c r="O17" s="42"/>
+      <c r="P17" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="58">
+      <c r="Q17" s="52">
         <v>6</v>
       </c>
-      <c r="R17" s="52" t="s">
+      <c r="R17" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="S17" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="S17" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T17" s="53" t="s">
-        <v>172</v>
-      </c>
-      <c r="U17" s="52" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T17" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="U17" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="W17" s="77">
+        <v>15</v>
+      </c>
+      <c r="X17" s="90" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>67</v>
       </c>
@@ -2670,51 +2898,57 @@
         <v>95</v>
       </c>
       <c r="F18" s="26"/>
-      <c r="G18" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="H18" s="13">
+      <c r="G18" s="78" t="s">
+        <v>206</v>
+      </c>
+      <c r="H18" s="79">
         <v>16</v>
       </c>
-      <c r="I18" s="28" t="s">
+      <c r="I18" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="J18" s="40" t="s">
-        <v>241</v>
+      <c r="J18" s="81" t="s">
+        <v>239</v>
       </c>
       <c r="K18" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L18" s="30" t="s">
+      <c r="L18" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M18" s="32"/>
-      <c r="N18" s="31" t="s">
+      <c r="M18" s="31"/>
+      <c r="N18" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="O18" s="45" t="s">
-        <v>239</v>
-      </c>
-      <c r="P18" s="54" t="s">
+      <c r="O18" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="P18" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="58">
+      <c r="Q18" s="52">
         <v>6</v>
       </c>
-      <c r="R18" s="52" t="s">
+      <c r="R18" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="S18" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="S18" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T18" s="53" t="s">
-        <v>240</v>
-      </c>
-      <c r="U18" s="52" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T18" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="U18" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="W18" s="77">
+        <v>16</v>
+      </c>
+      <c r="X18" s="90" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>67</v>
       </c>
@@ -2729,51 +2963,57 @@
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="26"/>
-      <c r="G19" s="27" t="s">
+      <c r="G19" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="79">
         <v>17</v>
       </c>
-      <c r="I19" s="47" t="s">
+      <c r="I19" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="J19" s="40" t="s">
-        <v>213</v>
+      <c r="J19" s="81" t="s">
+        <v>211</v>
       </c>
       <c r="K19" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L19" s="30" t="s">
+      <c r="L19" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="M19" s="32" t="s">
+      <c r="M19" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="N19" s="31"/>
-      <c r="O19" s="45" t="s">
-        <v>214</v>
-      </c>
-      <c r="P19" s="54" t="s">
+      <c r="N19" s="30"/>
+      <c r="O19" s="42" t="s">
+        <v>212</v>
+      </c>
+      <c r="P19" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="58">
+      <c r="Q19" s="52">
         <v>6</v>
       </c>
-      <c r="R19" s="56" t="s">
-        <v>186</v>
-      </c>
-      <c r="S19" s="56" t="s">
+      <c r="R19" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="S19" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="T19" s="54" t="s">
+        <v>213</v>
+      </c>
+      <c r="U19" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="T19" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="U19" s="56" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W19" s="77">
+        <v>17</v>
+      </c>
+      <c r="X19" s="90" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>67</v>
       </c>
@@ -2787,11 +3027,11 @@
         <v>115</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F20" s="26"/>
       <c r="G20" s="27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H20" s="13">
         <v>18</v>
@@ -2799,38 +3039,44 @@
       <c r="I20" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="J20" s="40" t="s">
-        <v>125</v>
+      <c r="J20" s="37" t="s">
+        <v>124</v>
       </c>
       <c r="K20" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L20" s="30" t="s">
+      <c r="L20" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="32"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="54" t="s">
+      <c r="M20" s="31"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="58">
+      <c r="Q20" s="52">
         <v>6</v>
       </c>
-      <c r="R20" s="52" t="s">
+      <c r="R20" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="S20" s="52" t="s">
+      <c r="S20" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="T20" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="U20" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="T20" s="52" t="s">
-        <v>126</v>
-      </c>
-      <c r="U20" s="52" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W20" s="77">
+        <v>18</v>
+      </c>
+      <c r="X20" s="90" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>67</v>
       </c>
@@ -2847,7 +3093,7 @@
         <v>116</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G21" s="27" t="s">
         <v>117</v>
@@ -2855,43 +3101,49 @@
       <c r="H21" s="13">
         <v>19</v>
       </c>
-      <c r="I21" s="48" t="s">
+      <c r="I21" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="J21" s="40" t="s">
-        <v>119</v>
+      <c r="J21" s="37" t="s">
+        <v>118</v>
       </c>
       <c r="K21" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L21" s="30" t="s">
+      <c r="L21" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M21" s="32"/>
-      <c r="N21" s="31" t="s">
+      <c r="M21" s="31"/>
+      <c r="N21" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="O21" s="45"/>
-      <c r="P21" s="54" t="s">
+      <c r="O21" s="42"/>
+      <c r="P21" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="58">
+      <c r="Q21" s="52">
         <v>6</v>
       </c>
-      <c r="R21" s="52" t="s">
+      <c r="R21" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="S21" s="52" t="s">
+      <c r="S21" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="T21" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="U21" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="T21" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="U21" s="52" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W21" s="77">
+        <v>19</v>
+      </c>
+      <c r="X21" s="90" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>67</v>
       </c>
@@ -2908,49 +3160,55 @@
         <v>116</v>
       </c>
       <c r="F22" s="26"/>
-      <c r="G22" s="29" t="s">
-        <v>217</v>
-      </c>
-      <c r="H22" s="13">
+      <c r="G22" s="95" t="s">
+        <v>215</v>
+      </c>
+      <c r="H22" s="87">
         <v>20</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="I22" s="87" t="s">
         <v>94</v>
       </c>
-      <c r="J22" s="50" t="s">
-        <v>218</v>
+      <c r="J22" s="96" t="s">
+        <v>216</v>
       </c>
       <c r="K22" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L22" s="30" t="s">
+      <c r="L22" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="M22" s="32"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="45" t="s">
-        <v>223</v>
-      </c>
-      <c r="P22" s="54" t="s">
+      <c r="M22" s="31"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="P22" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="58">
+      <c r="Q22" s="52">
         <v>6</v>
       </c>
-      <c r="R22" s="52" t="s">
+      <c r="R22" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="S22" s="52" t="s">
+      <c r="S22" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="T22" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="U22" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="T22" s="52" t="s">
-        <v>127</v>
-      </c>
-      <c r="U22" s="52" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W22" s="77">
+        <v>20</v>
+      </c>
+      <c r="X22" s="90" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>67</v>
       </c>
@@ -2964,11 +3222,11 @@
         <v>115</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F23" s="26"/>
       <c r="G23" s="27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H23" s="13">
         <v>21</v>
@@ -2976,40 +3234,46 @@
       <c r="I23" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J23" s="40" t="s">
-        <v>132</v>
+      <c r="J23" s="37" t="s">
+        <v>131</v>
       </c>
       <c r="K23" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L23" s="30" t="s">
+      <c r="L23" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="32"/>
-      <c r="N23" s="31" t="s">
+      <c r="M23" s="31"/>
+      <c r="N23" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="O23" s="45"/>
-      <c r="P23" s="54" t="s">
+      <c r="O23" s="42"/>
+      <c r="P23" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="58">
+      <c r="Q23" s="52">
         <v>6</v>
       </c>
-      <c r="R23" s="52" t="s">
+      <c r="R23" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="S23" s="52" t="s">
+      <c r="S23" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="T23" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="U23" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="T23" s="52" t="s">
-        <v>133</v>
-      </c>
-      <c r="U23" s="52" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W23" s="77">
+        <v>21</v>
+      </c>
+      <c r="X23" s="90" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>67</v>
       </c>
@@ -3023,11 +3287,11 @@
         <v>115</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F24" s="26"/>
       <c r="G24" s="27" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H24" s="13">
         <v>22</v>
@@ -3035,40 +3299,46 @@
       <c r="I24" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J24" s="40" t="s">
-        <v>135</v>
+      <c r="J24" s="37" t="s">
+        <v>134</v>
       </c>
       <c r="K24" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L24" s="30" t="s">
+      <c r="L24" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="32"/>
-      <c r="N24" s="31" t="s">
+      <c r="M24" s="31"/>
+      <c r="N24" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="O24" s="45"/>
-      <c r="P24" s="54" t="s">
+      <c r="O24" s="42"/>
+      <c r="P24" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="58">
+      <c r="Q24" s="52">
         <v>6</v>
       </c>
-      <c r="R24" s="52" t="s">
+      <c r="R24" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="S24" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="S24" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T24" s="53" t="s">
-        <v>173</v>
-      </c>
-      <c r="U24" s="52" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T24" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="U24" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="W24" s="76">
+        <v>22</v>
+      </c>
+      <c r="X24" s="90" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>67</v>
       </c>
@@ -3082,54 +3352,54 @@
         <v>115</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F25" s="26"/>
-      <c r="G25" s="27" t="s">
-        <v>219</v>
-      </c>
-      <c r="H25" s="13">
+      <c r="G25" s="78" t="s">
+        <v>217</v>
+      </c>
+      <c r="H25" s="79">
         <v>23</v>
       </c>
-      <c r="I25" s="28" t="s">
+      <c r="I25" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="J25" s="40" t="s">
-        <v>243</v>
+      <c r="J25" s="81" t="s">
+        <v>241</v>
       </c>
       <c r="K25" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L25" s="30" t="s">
+      <c r="L25" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M25" s="32"/>
-      <c r="N25" s="31" t="s">
+      <c r="M25" s="31"/>
+      <c r="N25" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="O25" s="45" t="s">
-        <v>244</v>
-      </c>
-      <c r="P25" s="54" t="s">
+      <c r="O25" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="P25" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="58">
+      <c r="Q25" s="52">
         <v>6</v>
       </c>
-      <c r="R25" s="52" t="s">
+      <c r="R25" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="S25" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="S25" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T25" s="53" t="s">
-        <v>245</v>
-      </c>
-      <c r="U25" s="52" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T25" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="U25" s="46" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>67</v>
       </c>
@@ -3140,14 +3410,14 @@
         <v>91</v>
       </c>
       <c r="D26" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>137</v>
       </c>
       <c r="F26" s="26"/>
       <c r="G26" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H26" s="13">
         <v>24</v>
@@ -3155,40 +3425,44 @@
       <c r="I26" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="J26" s="40" t="s">
-        <v>138</v>
+      <c r="J26" s="37" t="s">
+        <v>137</v>
       </c>
       <c r="K26" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L26" s="30" t="s">
+      <c r="L26" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="M26" s="32" t="s">
+      <c r="M26" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="N26" s="31"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="54" t="s">
+      <c r="N26" s="30"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="58">
+      <c r="Q26" s="52">
         <v>6</v>
       </c>
-      <c r="R26" s="52" t="s">
+      <c r="R26" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="S26" s="52" t="s">
+      <c r="S26" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="T26" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="T26" s="52" t="s">
+      <c r="U26" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="U26" s="52" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W26" s="91" t="s">
+        <v>259</v>
+      </c>
+      <c r="X26" s="92"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>67</v>
       </c>
@@ -3199,14 +3473,14 @@
         <v>91</v>
       </c>
       <c r="D27" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>137</v>
       </c>
       <c r="F27" s="26"/>
       <c r="G27" s="27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H27" s="13">
         <v>25</v>
@@ -3214,40 +3488,42 @@
       <c r="I27" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J27" s="40" t="s">
-        <v>146</v>
+      <c r="J27" s="37" t="s">
+        <v>145</v>
       </c>
       <c r="K27" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L27" s="30" t="s">
+      <c r="L27" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M27" s="32"/>
-      <c r="N27" s="31" t="s">
+      <c r="M27" s="31"/>
+      <c r="N27" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="O27" s="45"/>
-      <c r="P27" s="54" t="s">
+      <c r="O27" s="42"/>
+      <c r="P27" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="58">
+      <c r="Q27" s="52">
         <v>6</v>
       </c>
-      <c r="R27" s="52" t="s">
+      <c r="R27" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="S27" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="T27" s="52" t="s">
-        <v>147</v>
-      </c>
-      <c r="U27" s="52" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S27" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="T27" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="U27" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="W27" s="92"/>
+      <c r="X27" s="92"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>67</v>
       </c>
@@ -3258,14 +3534,14 @@
         <v>91</v>
       </c>
       <c r="D28" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>136</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>137</v>
       </c>
       <c r="F28" s="26"/>
       <c r="G28" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H28" s="13">
         <v>26</v>
@@ -3273,40 +3549,42 @@
       <c r="I28" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J28" s="40" t="s">
-        <v>149</v>
+      <c r="J28" s="37" t="s">
+        <v>148</v>
       </c>
       <c r="K28" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L28" s="30" t="s">
+      <c r="L28" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M28" s="32"/>
-      <c r="N28" s="31" t="s">
+      <c r="M28" s="31"/>
+      <c r="N28" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="O28" s="45"/>
-      <c r="P28" s="54" t="s">
+      <c r="O28" s="42"/>
+      <c r="P28" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="Q28" s="58">
+      <c r="Q28" s="52">
         <v>6</v>
       </c>
-      <c r="R28" s="52" t="s">
+      <c r="R28" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="S28" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="T28" s="52" t="s">
-        <v>148</v>
-      </c>
-      <c r="U28" s="52" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S28" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="T28" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="U28" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="W28" s="92"/>
+      <c r="X28" s="92"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>67</v>
       </c>
@@ -3317,14 +3595,14 @@
         <v>91</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F29" s="26"/>
       <c r="G29" s="27" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H29" s="13">
         <v>27</v>
@@ -3332,40 +3610,42 @@
       <c r="I29" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J29" s="40" t="s">
+      <c r="J29" s="37" t="s">
         <v>104</v>
       </c>
       <c r="K29" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L29" s="30" t="s">
+      <c r="L29" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M29" s="32"/>
-      <c r="N29" s="31" t="s">
+      <c r="M29" s="31"/>
+      <c r="N29" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="O29" s="45"/>
-      <c r="P29" s="54" t="s">
+      <c r="O29" s="42"/>
+      <c r="P29" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="58">
+      <c r="Q29" s="52">
         <v>6</v>
       </c>
-      <c r="R29" s="52" t="s">
+      <c r="R29" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="S29" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="T29" s="52" t="s">
-        <v>150</v>
-      </c>
-      <c r="U29" s="52" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S29" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="T29" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="U29" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="W29" s="92"/>
+      <c r="X29" s="92"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>67</v>
       </c>
@@ -3376,12 +3656,12 @@
         <v>91</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="26"/>
       <c r="G30" s="27" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H30" s="13">
         <v>28</v>
@@ -3389,40 +3669,42 @@
       <c r="I30" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J30" s="40" t="s">
-        <v>152</v>
+      <c r="J30" s="37" t="s">
+        <v>151</v>
       </c>
       <c r="K30" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L30" s="30" t="s">
+      <c r="L30" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M30" s="32"/>
-      <c r="N30" s="31" t="s">
+      <c r="M30" s="31"/>
+      <c r="N30" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="O30" s="45"/>
-      <c r="P30" s="54" t="s">
+      <c r="O30" s="42"/>
+      <c r="P30" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q30" s="58">
+      <c r="Q30" s="52">
         <v>6</v>
       </c>
-      <c r="R30" s="52" t="s">
+      <c r="R30" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="S30" s="52" t="s">
+      <c r="S30" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="T30" s="52" t="s">
-        <v>153</v>
-      </c>
-      <c r="U30" s="52" t="s">
+      <c r="T30" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="U30" s="46" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W30" s="92"/>
+      <c r="X30" s="92"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>67</v>
       </c>
@@ -3433,12 +3715,12 @@
         <v>91</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="26"/>
       <c r="G31" s="27" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H31" s="13">
         <v>29</v>
@@ -3446,40 +3728,42 @@
       <c r="I31" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J31" s="40" t="s">
-        <v>154</v>
+      <c r="J31" s="37" t="s">
+        <v>153</v>
       </c>
       <c r="K31" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L31" s="30" t="s">
+      <c r="L31" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M31" s="32"/>
-      <c r="N31" s="31" t="s">
+      <c r="M31" s="31"/>
+      <c r="N31" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="O31" s="45"/>
-      <c r="P31" s="54" t="s">
+      <c r="O31" s="42"/>
+      <c r="P31" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q31" s="58">
+      <c r="Q31" s="52">
         <v>6</v>
       </c>
-      <c r="R31" s="52" t="s">
+      <c r="R31" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="S31" s="52" t="s">
+      <c r="S31" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="T31" s="52" t="s">
-        <v>155</v>
-      </c>
-      <c r="U31" s="52" t="s">
+      <c r="T31" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="U31" s="46" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W31" s="92"/>
+      <c r="X31" s="92"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>67</v>
       </c>
@@ -3490,12 +3774,12 @@
         <v>91</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="26"/>
       <c r="G32" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H32" s="13">
         <v>30</v>
@@ -3503,26 +3787,26 @@
       <c r="I32" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J32" s="40" t="s">
-        <v>157</v>
+      <c r="J32" s="37" t="s">
+        <v>156</v>
       </c>
       <c r="K32" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L32" s="30" t="s">
+      <c r="L32" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="M32" s="32"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="54" t="s">
+      <c r="M32" s="31"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" s="51"/>
-      <c r="R32" s="52"/>
-      <c r="S32" s="52"/>
-      <c r="T32" s="52"/>
-      <c r="U32" s="52"/>
+      <c r="Q32" s="45"/>
+      <c r="R32" s="46"/>
+      <c r="S32" s="46"/>
+      <c r="T32" s="46"/>
+      <c r="U32" s="46"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
@@ -3535,12 +3819,12 @@
         <v>91</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="26"/>
       <c r="G33" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H33" s="13">
         <v>31</v>
@@ -3548,37 +3832,37 @@
       <c r="I33" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="J33" s="40" t="s">
-        <v>159</v>
+      <c r="J33" s="37" t="s">
+        <v>158</v>
       </c>
       <c r="K33" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L33" s="30" t="s">
+      <c r="L33" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M33" s="32"/>
-      <c r="N33" s="31" t="s">
+      <c r="M33" s="31"/>
+      <c r="N33" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="O33" s="45"/>
-      <c r="P33" s="54" t="s">
+      <c r="O33" s="42"/>
+      <c r="P33" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="Q33" s="61">
+      <c r="Q33" s="55">
         <v>6</v>
       </c>
-      <c r="R33" s="52" t="s">
+      <c r="R33" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="S33" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="S33" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T33" s="53" t="s">
-        <v>174</v>
-      </c>
-      <c r="U33" s="52" t="s">
-        <v>168</v>
+      <c r="T33" s="47" t="s">
+        <v>173</v>
+      </c>
+      <c r="U33" s="46" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -3592,59 +3876,72 @@
         <v>91</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="26"/>
-      <c r="G34" s="27" t="s">
-        <v>227</v>
-      </c>
-      <c r="H34" s="13">
+      <c r="G34" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="H34" s="79">
         <v>32</v>
       </c>
-      <c r="I34" s="28" t="s">
+      <c r="I34" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="J34" s="40" t="s">
-        <v>227</v>
+      <c r="J34" s="81" t="s">
+        <v>225</v>
       </c>
       <c r="K34" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="L34" s="30" t="s">
+      <c r="L34" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="M34" s="32"/>
-      <c r="N34" s="31" t="s">
+      <c r="M34" s="31"/>
+      <c r="N34" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="O34" s="45"/>
-      <c r="P34" s="54" t="s">
+      <c r="O34" s="42"/>
+      <c r="P34" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="Q34" s="61">
+      <c r="Q34" s="55">
         <v>6</v>
       </c>
-      <c r="R34" s="52" t="s">
+      <c r="R34" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="S34" s="46" t="s">
         <v>165</v>
       </c>
-      <c r="S34" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="T34" s="53" t="s">
-        <v>226</v>
-      </c>
-      <c r="U34" s="52" t="s">
-        <v>168</v>
-      </c>
+      <c r="T34" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="U34" s="46" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="93" t="s">
+        <v>260</v>
+      </c>
+      <c r="B36" s="94"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="94"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="97" t="s">
+        <v>261</v>
+      </c>
+      <c r="B37" s="98"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="98"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
+  <mergeCells count="22">
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="W26:X31"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -3660,6 +3957,11 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4371,40 +4673,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="75" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" s="67" t="s">
+      <c r="G1" s="70" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="62" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="68"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="77"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -4422,10 +4724,10 @@
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
       <c r="G3" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4442,11 +4744,11 @@
         <v>115</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H4" s="15"/>
     </row>
@@ -4502,20 +4804,17 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>177</v>
-      </c>
-      <c r="G1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" t="s">
         <v>180</v>
-      </c>
-      <c r="K1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -4525,41 +4824,33 @@
       <c r="B3" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>144</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -4568,10 +4859,10 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -4580,10 +4871,10 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrección títulos mapas conceptuales
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/ESCALETA_CN_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/ESCALETA_CN_08_04_CO.xlsx
@@ -1372,60 +1372,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1463,12 +1409,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1477,6 +1417,66 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1760,8 +1760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,102 +1791,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="62" t="s">
+      <c r="H1" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="60" t="s">
+      <c r="I1" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="K1" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="62" t="s">
+      <c r="L1" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="66" t="s">
+      <c r="M1" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="60" t="s">
+      <c r="N1" s="93"/>
+      <c r="O1" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="62" t="s">
+      <c r="P1" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="58" t="s">
+      <c r="Q1" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="62" t="s">
+      <c r="R1" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="64" t="s">
+      <c r="S1" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="62" t="s">
+      <c r="T1" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="64" t="s">
+      <c r="U1" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="73" t="s">
+      <c r="W1" s="87" t="s">
         <v>247</v>
       </c>
-      <c r="X1" s="73"/>
+      <c r="X1" s="87"/>
     </row>
     <row r="2" spans="1:24" s="7" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="59"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="63"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="82"/>
       <c r="M2" s="23" t="s">
         <v>87</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="61"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="65"/>
-      <c r="W2" s="74" t="s">
+      <c r="O2" s="86"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="91"/>
+      <c r="W2" s="56" t="s">
         <v>248</v>
       </c>
-      <c r="X2" s="75" t="s">
+      <c r="X2" s="57" t="s">
         <v>249</v>
       </c>
     </row>
@@ -1907,16 +1907,16 @@
         <v>159</v>
       </c>
       <c r="F3" s="26"/>
-      <c r="G3" s="78" t="s">
+      <c r="G3" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="79">
+      <c r="H3" s="61">
         <v>1</v>
       </c>
-      <c r="I3" s="80" t="s">
+      <c r="I3" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="J3" s="81" t="s">
+      <c r="J3" s="63" t="s">
         <v>188</v>
       </c>
       <c r="K3" s="14" t="s">
@@ -1950,10 +1950,10 @@
       <c r="U3" s="49" t="s">
         <v>187</v>
       </c>
-      <c r="W3" s="76">
+      <c r="W3" s="58">
         <v>1</v>
       </c>
-      <c r="X3" s="90" t="s">
+      <c r="X3" s="72" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1974,16 +1974,16 @@
         <v>159</v>
       </c>
       <c r="F4" s="26"/>
-      <c r="G4" s="78" t="s">
+      <c r="G4" s="60" t="s">
         <v>226</v>
       </c>
-      <c r="H4" s="79">
+      <c r="H4" s="61">
         <v>2</v>
       </c>
-      <c r="I4" s="82" t="s">
+      <c r="I4" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="J4" s="81" t="s">
+      <c r="J4" s="63" t="s">
         <v>189</v>
       </c>
       <c r="K4" s="14" t="s">
@@ -2017,10 +2017,10 @@
       <c r="U4" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="W4" s="76">
+      <c r="W4" s="58">
         <v>2</v>
       </c>
-      <c r="X4" s="90" t="s">
+      <c r="X4" s="72" t="s">
         <v>250</v>
       </c>
     </row>
@@ -2041,16 +2041,16 @@
         <v>95</v>
       </c>
       <c r="F5" s="26"/>
-      <c r="G5" s="78" t="s">
+      <c r="G5" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="H5" s="79">
+      <c r="H5" s="61">
         <v>3</v>
       </c>
-      <c r="I5" s="79" t="s">
+      <c r="I5" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="J5" s="83" t="s">
+      <c r="J5" s="65" t="s">
         <v>190</v>
       </c>
       <c r="K5" s="14" t="s">
@@ -2084,10 +2084,10 @@
       <c r="U5" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="W5" s="76">
+      <c r="W5" s="58">
         <v>3</v>
       </c>
-      <c r="X5" s="90" t="s">
+      <c r="X5" s="72" t="s">
         <v>251</v>
       </c>
     </row>
@@ -2149,10 +2149,10 @@
       <c r="U6" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="W6" s="76">
+      <c r="W6" s="58">
         <v>4</v>
       </c>
-      <c r="X6" s="90" t="s">
+      <c r="X6" s="72" t="s">
         <v>252</v>
       </c>
     </row>
@@ -2171,16 +2171,16 @@
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="26"/>
-      <c r="G7" s="78" t="s">
+      <c r="G7" s="60" t="s">
         <v>178</v>
       </c>
-      <c r="H7" s="79">
+      <c r="H7" s="61">
         <v>5</v>
       </c>
-      <c r="I7" s="80" t="s">
+      <c r="I7" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="J7" s="81" t="s">
+      <c r="J7" s="63" t="s">
         <v>196</v>
       </c>
       <c r="K7" s="14" t="s">
@@ -2214,10 +2214,10 @@
       <c r="U7" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="W7" s="76">
+      <c r="W7" s="58">
         <v>5</v>
       </c>
-      <c r="X7" s="90" t="s">
+      <c r="X7" s="72" t="s">
         <v>254</v>
       </c>
     </row>
@@ -2281,10 +2281,10 @@
       <c r="U8" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="W8" s="76">
+      <c r="W8" s="58">
         <v>6</v>
       </c>
-      <c r="X8" s="90" t="s">
+      <c r="X8" s="72" t="s">
         <v>253</v>
       </c>
     </row>
@@ -2307,16 +2307,16 @@
       <c r="F9" s="36" t="s">
         <v>227</v>
       </c>
-      <c r="G9" s="84" t="s">
+      <c r="G9" s="66" t="s">
         <v>174</v>
       </c>
-      <c r="H9" s="79">
+      <c r="H9" s="61">
         <v>7</v>
       </c>
-      <c r="I9" s="80" t="s">
+      <c r="I9" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="J9" s="81" t="s">
+      <c r="J9" s="63" t="s">
         <v>198</v>
       </c>
       <c r="K9" s="38" t="s">
@@ -2350,10 +2350,10 @@
       <c r="U9" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="W9" s="76">
+      <c r="W9" s="58">
         <v>7</v>
       </c>
-      <c r="X9" s="90" t="s">
+      <c r="X9" s="72" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2417,10 +2417,10 @@
       <c r="U10" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="W10" s="77">
+      <c r="W10" s="59">
         <v>8</v>
       </c>
-      <c r="X10" s="90" t="s">
+      <c r="X10" s="72" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2441,16 +2441,16 @@
         <v>95</v>
       </c>
       <c r="F11" s="36"/>
-      <c r="G11" s="78" t="s">
+      <c r="G11" s="60" t="s">
         <v>228</v>
       </c>
-      <c r="H11" s="79">
+      <c r="H11" s="61">
         <v>9</v>
       </c>
-      <c r="I11" s="80" t="s">
+      <c r="I11" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="J11" s="81" t="s">
+      <c r="J11" s="63" t="s">
         <v>229</v>
       </c>
       <c r="K11" s="14" t="s">
@@ -2484,10 +2484,10 @@
       <c r="U11" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="W11" s="77">
+      <c r="W11" s="59">
         <v>9</v>
       </c>
-      <c r="X11" s="90" t="s">
+      <c r="X11" s="72" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2508,16 +2508,16 @@
         <v>204</v>
       </c>
       <c r="F12" s="26"/>
-      <c r="G12" s="78" t="s">
+      <c r="G12" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="H12" s="79">
+      <c r="H12" s="61">
         <v>10</v>
       </c>
-      <c r="I12" s="80" t="s">
+      <c r="I12" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="J12" s="81" t="s">
+      <c r="J12" s="63" t="s">
         <v>201</v>
       </c>
       <c r="K12" s="14" t="s">
@@ -2551,10 +2551,10 @@
       <c r="U12" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="W12" s="77">
+      <c r="W12" s="59">
         <v>10</v>
       </c>
-      <c r="X12" s="90" t="s">
+      <c r="X12" s="72" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2616,10 +2616,10 @@
       <c r="U13" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="W13" s="77">
+      <c r="W13" s="59">
         <v>11</v>
       </c>
-      <c r="X13" s="90" t="s">
+      <c r="X13" s="72" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2640,16 +2640,16 @@
         <v>95</v>
       </c>
       <c r="F14" s="26"/>
-      <c r="G14" s="78" t="s">
+      <c r="G14" s="60" t="s">
         <v>205</v>
       </c>
-      <c r="H14" s="79">
+      <c r="H14" s="61">
         <v>12</v>
       </c>
-      <c r="I14" s="80" t="s">
+      <c r="I14" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="J14" s="81" t="s">
+      <c r="J14" s="63" t="s">
         <v>246</v>
       </c>
       <c r="K14" s="14" t="s">
@@ -2683,10 +2683,10 @@
       <c r="U14" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="W14" s="77">
+      <c r="W14" s="59">
         <v>12</v>
       </c>
-      <c r="X14" s="90" t="s">
+      <c r="X14" s="72" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2705,16 +2705,16 @@
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="26"/>
-      <c r="G15" s="78" t="s">
+      <c r="G15" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="H15" s="79">
+      <c r="H15" s="61">
         <v>13</v>
       </c>
-      <c r="I15" s="80" t="s">
+      <c r="I15" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="J15" s="81" t="s">
+      <c r="J15" s="63" t="s">
         <v>207</v>
       </c>
       <c r="K15" s="14" t="s">
@@ -2748,10 +2748,10 @@
       <c r="U15" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="W15" s="77">
+      <c r="W15" s="59">
         <v>13</v>
       </c>
-      <c r="X15" s="90" t="s">
+      <c r="X15" s="72" t="s">
         <v>256</v>
       </c>
     </row>
@@ -2770,16 +2770,16 @@
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="26"/>
-      <c r="G16" s="86" t="s">
+      <c r="G16" s="68" t="s">
         <v>245</v>
       </c>
-      <c r="H16" s="87">
+      <c r="H16" s="69">
         <v>14</v>
       </c>
-      <c r="I16" s="88" t="s">
+      <c r="I16" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="J16" s="89" t="s">
+      <c r="J16" s="71" t="s">
         <v>210</v>
       </c>
       <c r="K16" s="14" t="s">
@@ -2811,10 +2811,10 @@
       <c r="U16" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="W16" s="77">
+      <c r="W16" s="59">
         <v>14</v>
       </c>
-      <c r="X16" s="90" t="s">
+      <c r="X16" s="72" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2874,10 +2874,10 @@
       <c r="U17" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="W17" s="77">
+      <c r="W17" s="59">
         <v>15</v>
       </c>
-      <c r="X17" s="90" t="s">
+      <c r="X17" s="72" t="s">
         <v>257</v>
       </c>
     </row>
@@ -2898,16 +2898,16 @@
         <v>95</v>
       </c>
       <c r="F18" s="26"/>
-      <c r="G18" s="78" t="s">
+      <c r="G18" s="60" t="s">
         <v>206</v>
       </c>
-      <c r="H18" s="79">
+      <c r="H18" s="61">
         <v>16</v>
       </c>
-      <c r="I18" s="80" t="s">
+      <c r="I18" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="J18" s="81" t="s">
+      <c r="J18" s="63" t="s">
         <v>239</v>
       </c>
       <c r="K18" s="14" t="s">
@@ -2941,10 +2941,10 @@
       <c r="U18" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="W18" s="77">
+      <c r="W18" s="59">
         <v>16</v>
       </c>
-      <c r="X18" s="90" t="s">
+      <c r="X18" s="72" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2963,16 +2963,16 @@
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="26"/>
-      <c r="G19" s="78" t="s">
+      <c r="G19" s="60" t="s">
         <v>115</v>
       </c>
-      <c r="H19" s="79">
+      <c r="H19" s="61">
         <v>17</v>
       </c>
-      <c r="I19" s="85" t="s">
+      <c r="I19" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="J19" s="81" t="s">
+      <c r="J19" s="63" t="s">
         <v>211</v>
       </c>
       <c r="K19" s="14" t="s">
@@ -3006,10 +3006,10 @@
       <c r="U19" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="W19" s="77">
+      <c r="W19" s="59">
         <v>17</v>
       </c>
-      <c r="X19" s="90" t="s">
+      <c r="X19" s="72" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3069,10 +3069,10 @@
       <c r="U20" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="W20" s="77">
+      <c r="W20" s="59">
         <v>18</v>
       </c>
-      <c r="X20" s="90" t="s">
+      <c r="X20" s="72" t="s">
         <v>149</v>
       </c>
     </row>
@@ -3136,10 +3136,10 @@
       <c r="U21" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="W21" s="77">
+      <c r="W21" s="59">
         <v>19</v>
       </c>
-      <c r="X21" s="90" t="s">
+      <c r="X21" s="72" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3160,16 +3160,16 @@
         <v>116</v>
       </c>
       <c r="F22" s="26"/>
-      <c r="G22" s="95" t="s">
+      <c r="G22" s="75" t="s">
         <v>215</v>
       </c>
-      <c r="H22" s="87">
+      <c r="H22" s="69">
         <v>20</v>
       </c>
-      <c r="I22" s="87" t="s">
+      <c r="I22" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="J22" s="96" t="s">
+      <c r="J22" s="76" t="s">
         <v>216</v>
       </c>
       <c r="K22" s="14" t="s">
@@ -3201,10 +3201,10 @@
       <c r="U22" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="W22" s="77">
+      <c r="W22" s="59">
         <v>20</v>
       </c>
-      <c r="X22" s="90" t="s">
+      <c r="X22" s="72" t="s">
         <v>258</v>
       </c>
     </row>
@@ -3266,10 +3266,10 @@
       <c r="U23" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="W23" s="77">
+      <c r="W23" s="59">
         <v>21</v>
       </c>
-      <c r="X23" s="90" t="s">
+      <c r="X23" s="72" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3331,10 +3331,10 @@
       <c r="U24" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="W24" s="76">
+      <c r="W24" s="58">
         <v>22</v>
       </c>
-      <c r="X24" s="90" t="s">
+      <c r="X24" s="72" t="s">
         <v>157</v>
       </c>
     </row>
@@ -3355,16 +3355,16 @@
         <v>133</v>
       </c>
       <c r="F25" s="26"/>
-      <c r="G25" s="78" t="s">
+      <c r="G25" s="60" t="s">
         <v>217</v>
       </c>
-      <c r="H25" s="79">
+      <c r="H25" s="61">
         <v>23</v>
       </c>
-      <c r="I25" s="80" t="s">
+      <c r="I25" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="J25" s="81" t="s">
+      <c r="J25" s="63" t="s">
         <v>241</v>
       </c>
       <c r="K25" s="14" t="s">
@@ -3457,10 +3457,10 @@
       <c r="U26" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="W26" s="91" t="s">
+      <c r="W26" s="88" t="s">
         <v>259</v>
       </c>
-      <c r="X26" s="92"/>
+      <c r="X26" s="89"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
@@ -3520,8 +3520,8 @@
       <c r="U27" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="W27" s="92"/>
-      <c r="X27" s="92"/>
+      <c r="W27" s="89"/>
+      <c r="X27" s="89"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
@@ -3581,8 +3581,8 @@
       <c r="U28" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="W28" s="92"/>
-      <c r="X28" s="92"/>
+      <c r="W28" s="89"/>
+      <c r="X28" s="89"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
@@ -3642,8 +3642,8 @@
       <c r="U29" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="W29" s="92"/>
-      <c r="X29" s="92"/>
+      <c r="W29" s="89"/>
+      <c r="X29" s="89"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
@@ -3701,8 +3701,8 @@
       <c r="U30" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="W30" s="92"/>
-      <c r="X30" s="92"/>
+      <c r="W30" s="89"/>
+      <c r="X30" s="89"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
@@ -3760,8 +3760,8 @@
       <c r="U31" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="W31" s="92"/>
-      <c r="X31" s="92"/>
+      <c r="W31" s="89"/>
+      <c r="X31" s="89"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
@@ -3880,16 +3880,16 @@
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="26"/>
-      <c r="G34" s="78" t="s">
+      <c r="G34" s="60" t="s">
         <v>225</v>
       </c>
-      <c r="H34" s="79">
+      <c r="H34" s="61">
         <v>32</v>
       </c>
-      <c r="I34" s="80" t="s">
+      <c r="I34" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="J34" s="81" t="s">
+      <c r="J34" s="63" t="s">
         <v>225</v>
       </c>
       <c r="K34" s="14" t="s">
@@ -3923,20 +3923,20 @@
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="93" t="s">
+      <c r="A36" s="73" t="s">
         <v>260</v>
       </c>
-      <c r="B36" s="94"/>
-      <c r="C36" s="94"/>
-      <c r="D36" s="94"/>
+      <c r="B36" s="74"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="74"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="97" t="s">
+      <c r="A37" s="77" t="s">
         <v>261</v>
       </c>
-      <c r="B37" s="98"/>
-      <c r="C37" s="98"/>
-      <c r="D37" s="98"/>
+      <c r="B37" s="78"/>
+      <c r="C37" s="78"/>
+      <c r="D37" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -3956,12 +3956,12 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4673,40 +4673,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="62" t="s">
+      <c r="H1" s="81" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="72"/>
+      <c r="A2" s="82"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="98"/>
     </row>
     <row r="3" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">

</xml_diff>

<commit_message>
Corrección mayúsculas después de punto
Se arreglan las mayúsculas en los Refuerza tu aprendizaje
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/ESCALETA_CN_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/ESCALETA_CN_08_04_CO.xlsx
@@ -12,7 +12,7 @@
     <sheet name="VER" sheetId="3" r:id="rId3"/>
     <sheet name="Recursos alterados" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="261">
   <si>
     <t>Asignatura</t>
   </si>
@@ -549,9 +549,6 @@
     <t>La reproducción sexual de los seres vivos</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: la importancia de la reproducción</t>
-  </si>
-  <si>
     <t>Recursos eliminados que se propusieron</t>
   </si>
   <si>
@@ -639,12 +636,6 @@
     <t>La reproducción de protistas</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: la reproducción de los microorganismos</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: la reproducción de los hongos</t>
-  </si>
-  <si>
     <t>Interactivo que permite conocer la reproducción de los hongos</t>
   </si>
   <si>
@@ -675,12 +666,6 @@
     <t>Animación que muestra la reproducción sexual de las plantas con flor</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: la reproducción de las plantas</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: la reproducción de los animales</t>
-  </si>
-  <si>
     <t>Competencias: relaciona los tipos de reproducción con organismos en los que se lleva a cabo</t>
   </si>
   <si>
@@ -708,9 +693,6 @@
     <t>Ventajas y desventajas de la reproducción sexual</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: los tipos de reproducción en la naturaleza</t>
-  </si>
-  <si>
     <t>Actividad acerca de los tipos de reproducción en la naturaleza</t>
   </si>
   <si>
@@ -810,7 +792,19 @@
     <t>Los recursos en naranja son unos que ya están montados pero que requieren cambios importantes: el audio en los videos</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: la reproducción y las estrategias reproductivas</t>
+    <t>Refuerza tu aprendizaje: La reproducción y las estrategias reproductivas</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La importancia de la reproducción</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Los tipos de reproducción en la naturaleza</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La reproducción de los microorganismos</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La reproducción de los animales</t>
   </si>
 </sst>
 </file>
@@ -1420,6 +1414,30 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1429,12 +1447,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1447,29 +1459,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1753,7 +1747,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1763,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,103 +1788,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="82" t="s">
+      <c r="D1" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="94" t="s">
+      <c r="E1" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="84" t="s">
+      <c r="F1" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="82" t="s">
+      <c r="G1" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="88" t="s">
+      <c r="H1" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="90" t="s">
+      <c r="I1" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="88" t="s">
+      <c r="J1" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="92" t="s">
+      <c r="K1" s="94" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="88" t="s">
+      <c r="L1" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="86" t="s">
+      <c r="M1" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="87"/>
-      <c r="O1" s="90" t="s">
+      <c r="N1" s="93"/>
+      <c r="O1" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="88" t="s">
+      <c r="P1" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="82" t="s">
+      <c r="Q1" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="88" t="s">
+      <c r="R1" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="84" t="s">
+      <c r="S1" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="88" t="s">
+      <c r="T1" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="84" t="s">
+      <c r="U1" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="79" t="s">
-        <v>247</v>
-      </c>
-      <c r="X1" s="79"/>
+      <c r="W1" s="87" t="s">
+        <v>241</v>
+      </c>
+      <c r="X1" s="87"/>
     </row>
     <row r="2" spans="1:24" s="7" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="83"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="89"/>
+      <c r="A2" s="80"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="82"/>
       <c r="M2" s="23" t="s">
         <v>87</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="91"/>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="85"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="85"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="91"/>
       <c r="W2" s="56" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="X2" s="57" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1920,7 +1914,7 @@
         <v>94</v>
       </c>
       <c r="J3" s="63" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>69</v>
@@ -1933,7 +1927,7 @@
       </c>
       <c r="N3" s="30"/>
       <c r="O3" s="42" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P3" s="48" t="s">
         <v>19</v>
@@ -1942,16 +1936,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="49" t="s">
+        <v>183</v>
+      </c>
+      <c r="S3" s="49" t="s">
         <v>184</v>
       </c>
-      <c r="S3" s="49" t="s">
+      <c r="T3" s="53" t="s">
         <v>185</v>
       </c>
-      <c r="T3" s="53" t="s">
+      <c r="U3" s="49" t="s">
         <v>186</v>
-      </c>
-      <c r="U3" s="49" t="s">
-        <v>187</v>
       </c>
       <c r="W3" s="58">
         <v>1</v>
@@ -1978,7 +1972,7 @@
       </c>
       <c r="F4" s="26"/>
       <c r="G4" s="60" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="H4" s="61">
         <v>2</v>
@@ -1987,7 +1981,7 @@
         <v>96</v>
       </c>
       <c r="J4" s="63" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>69</v>
@@ -2000,7 +1994,7 @@
         <v>24</v>
       </c>
       <c r="O4" s="42" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P4" s="48" t="s">
         <v>19</v>
@@ -2024,7 +2018,7 @@
         <v>2</v>
       </c>
       <c r="X4" s="72" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2045,7 +2039,7 @@
       </c>
       <c r="F5" s="26"/>
       <c r="G5" s="60" t="s">
-        <v>175</v>
+        <v>257</v>
       </c>
       <c r="H5" s="61">
         <v>3</v>
@@ -2054,7 +2048,7 @@
         <v>96</v>
       </c>
       <c r="J5" s="65" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>69</v>
@@ -2067,7 +2061,7 @@
         <v>62</v>
       </c>
       <c r="O5" s="42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P5" s="48" t="s">
         <v>20</v>
@@ -2091,7 +2085,7 @@
         <v>3</v>
       </c>
       <c r="X5" s="72" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2112,7 +2106,7 @@
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="27" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="H6" s="13">
         <v>4</v>
@@ -2121,7 +2115,7 @@
         <v>96</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>69</v>
@@ -2147,7 +2141,7 @@
         <v>165</v>
       </c>
       <c r="T6" s="47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="U6" s="46" t="s">
         <v>167</v>
@@ -2156,7 +2150,7 @@
         <v>4</v>
       </c>
       <c r="X6" s="72" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2175,7 +2169,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="26"/>
       <c r="G7" s="60" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H7" s="61">
         <v>5</v>
@@ -2184,7 +2178,7 @@
         <v>94</v>
       </c>
       <c r="J7" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>69</v>
@@ -2197,7 +2191,7 @@
       </c>
       <c r="N7" s="30"/>
       <c r="O7" s="42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P7" s="48" t="s">
         <v>19</v>
@@ -2206,22 +2200,22 @@
         <v>6</v>
       </c>
       <c r="R7" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="S7" s="50" t="s">
         <v>184</v>
       </c>
-      <c r="S7" s="50" t="s">
-        <v>185</v>
-      </c>
       <c r="T7" s="54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="U7" s="50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="W7" s="58">
         <v>5</v>
       </c>
       <c r="X7" s="72" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -2288,7 +2282,7 @@
         <v>6</v>
       </c>
       <c r="X8" s="72" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:24" s="43" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2305,10 +2299,10 @@
         <v>97</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="G9" s="66" t="s">
         <v>174</v>
@@ -2320,7 +2314,7 @@
         <v>96</v>
       </c>
       <c r="J9" s="63" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K9" s="38" t="s">
         <v>69</v>
@@ -2333,7 +2327,7 @@
         <v>60</v>
       </c>
       <c r="O9" s="42" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P9" s="48" t="s">
         <v>19</v>
@@ -2348,7 +2342,7 @@
         <v>165</v>
       </c>
       <c r="T9" s="47" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="U9" s="46" t="s">
         <v>167</v>
@@ -2374,13 +2368,13 @@
         <v>97</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="H10" s="13">
         <v>8</v>
@@ -2415,7 +2409,7 @@
         <v>165</v>
       </c>
       <c r="T10" s="47" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="U10" s="46" t="s">
         <v>167</v>
@@ -2424,7 +2418,7 @@
         <v>8</v>
       </c>
       <c r="X10" s="72" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -2445,7 +2439,7 @@
       </c>
       <c r="F11" s="36"/>
       <c r="G11" s="60" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="H11" s="61">
         <v>9</v>
@@ -2454,7 +2448,7 @@
         <v>96</v>
       </c>
       <c r="J11" s="63" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="K11" s="14" t="s">
         <v>69</v>
@@ -2467,7 +2461,7 @@
         <v>62</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="P11" s="48" t="s">
         <v>19</v>
@@ -2482,7 +2476,7 @@
         <v>165</v>
       </c>
       <c r="T11" s="47" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="U11" s="46" t="s">
         <v>167</v>
@@ -2508,11 +2502,11 @@
         <v>109</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="60" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H12" s="61">
         <v>10</v>
@@ -2521,7 +2515,7 @@
         <v>94</v>
       </c>
       <c r="J12" s="63" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K12" s="14" t="s">
         <v>69</v>
@@ -2534,7 +2528,7 @@
       </c>
       <c r="N12" s="30"/>
       <c r="O12" s="42" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P12" s="48" t="s">
         <v>19</v>
@@ -2543,16 +2537,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="S12" s="50" t="s">
         <v>184</v>
       </c>
-      <c r="S12" s="50" t="s">
-        <v>185</v>
-      </c>
       <c r="T12" s="54" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U12" s="50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="W12" s="59">
         <v>10</v>
@@ -2575,11 +2569,11 @@
         <v>109</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="27" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="H13" s="13">
         <v>11</v>
@@ -2588,7 +2582,7 @@
         <v>96</v>
       </c>
       <c r="J13" s="37" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="K13" s="14" t="s">
         <v>69</v>
@@ -2644,7 +2638,7 @@
       </c>
       <c r="F14" s="26"/>
       <c r="G14" s="60" t="s">
-        <v>205</v>
+        <v>259</v>
       </c>
       <c r="H14" s="61">
         <v>12</v>
@@ -2653,7 +2647,7 @@
         <v>96</v>
       </c>
       <c r="J14" s="63" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="K14" s="14" t="s">
         <v>69</v>
@@ -2666,7 +2660,7 @@
         <v>62</v>
       </c>
       <c r="O14" s="42" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="P14" s="48" t="s">
         <v>19</v>
@@ -2681,7 +2675,7 @@
         <v>165</v>
       </c>
       <c r="T14" s="47" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="U14" s="46" t="s">
         <v>167</v>
@@ -2718,7 +2712,7 @@
         <v>94</v>
       </c>
       <c r="J15" s="63" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K15" s="14" t="s">
         <v>69</v>
@@ -2731,7 +2725,7 @@
       </c>
       <c r="N15" s="30"/>
       <c r="O15" s="42" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="P15" s="48" t="s">
         <v>19</v>
@@ -2740,22 +2734,22 @@
         <v>6</v>
       </c>
       <c r="R15" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="S15" s="50" t="s">
         <v>184</v>
       </c>
-      <c r="S15" s="50" t="s">
-        <v>185</v>
-      </c>
       <c r="T15" s="54" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="U15" s="50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="W15" s="59">
         <v>13</v>
       </c>
       <c r="X15" s="72" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -2774,7 +2768,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="26"/>
       <c r="G16" s="68" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="H16" s="69">
         <v>14</v>
@@ -2783,7 +2777,7 @@
         <v>94</v>
       </c>
       <c r="J16" s="71" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K16" s="14" t="s">
         <v>70</v>
@@ -2794,7 +2788,7 @@
       <c r="M16" s="31"/>
       <c r="N16" s="30"/>
       <c r="O16" s="42" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="P16" s="48" t="s">
         <v>19</v>
@@ -2837,7 +2831,7 @@
       <c r="E17" s="12"/>
       <c r="F17" s="26"/>
       <c r="G17" s="27" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="H17" s="13">
         <v>15</v>
@@ -2881,7 +2875,7 @@
         <v>15</v>
       </c>
       <c r="X17" s="72" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -2902,7 +2896,7 @@
       </c>
       <c r="F18" s="26"/>
       <c r="G18" s="60" t="s">
-        <v>206</v>
+        <v>249</v>
       </c>
       <c r="H18" s="61">
         <v>16</v>
@@ -2911,7 +2905,7 @@
         <v>96</v>
       </c>
       <c r="J18" s="63" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="K18" s="14" t="s">
         <v>69</v>
@@ -2924,7 +2918,7 @@
         <v>62</v>
       </c>
       <c r="O18" s="42" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="P18" s="48" t="s">
         <v>19</v>
@@ -2939,7 +2933,7 @@
         <v>165</v>
       </c>
       <c r="T18" s="47" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="U18" s="46" t="s">
         <v>167</v>
@@ -2976,7 +2970,7 @@
         <v>94</v>
       </c>
       <c r="J19" s="63" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K19" s="14" t="s">
         <v>69</v>
@@ -2989,7 +2983,7 @@
       </c>
       <c r="N19" s="30"/>
       <c r="O19" s="42" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P19" s="48" t="s">
         <v>19</v>
@@ -2998,16 +2992,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="S19" s="50" t="s">
         <v>184</v>
       </c>
-      <c r="S19" s="50" t="s">
-        <v>185</v>
-      </c>
       <c r="T19" s="54" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="U19" s="50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="W19" s="59">
         <v>17</v>
@@ -3030,11 +3024,11 @@
         <v>115</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F20" s="26"/>
       <c r="G20" s="27" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H20" s="13">
         <v>18</v>
@@ -3164,7 +3158,7 @@
       </c>
       <c r="F22" s="26"/>
       <c r="G22" s="75" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H22" s="69">
         <v>20</v>
@@ -3173,7 +3167,7 @@
         <v>94</v>
       </c>
       <c r="J22" s="76" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="K22" s="14" t="s">
         <v>70</v>
@@ -3184,7 +3178,7 @@
       <c r="M22" s="31"/>
       <c r="N22" s="30"/>
       <c r="O22" s="42" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="P22" s="48" t="s">
         <v>19</v>
@@ -3208,7 +3202,7 @@
         <v>20</v>
       </c>
       <c r="X22" s="72" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -3229,7 +3223,7 @@
       </c>
       <c r="F23" s="26"/>
       <c r="G23" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H23" s="13">
         <v>21</v>
@@ -3294,7 +3288,7 @@
       </c>
       <c r="F24" s="26"/>
       <c r="G24" s="27" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="H24" s="13">
         <v>22</v>
@@ -3359,7 +3353,7 @@
       </c>
       <c r="F25" s="26"/>
       <c r="G25" s="60" t="s">
-        <v>217</v>
+        <v>250</v>
       </c>
       <c r="H25" s="61">
         <v>23</v>
@@ -3368,7 +3362,7 @@
         <v>96</v>
       </c>
       <c r="J25" s="63" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="K25" s="14" t="s">
         <v>69</v>
@@ -3381,7 +3375,7 @@
         <v>62</v>
       </c>
       <c r="O25" s="42" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="P25" s="48" t="s">
         <v>19</v>
@@ -3396,7 +3390,7 @@
         <v>165</v>
       </c>
       <c r="T25" s="47" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="U25" s="46" t="s">
         <v>167</v>
@@ -3460,10 +3454,10 @@
       <c r="U26" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="W26" s="80" t="s">
-        <v>259</v>
-      </c>
-      <c r="X26" s="81"/>
+      <c r="W26" s="88" t="s">
+        <v>253</v>
+      </c>
+      <c r="X26" s="89"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
@@ -3483,7 +3477,7 @@
       </c>
       <c r="F27" s="26"/>
       <c r="G27" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H27" s="13">
         <v>25</v>
@@ -3523,8 +3517,8 @@
       <c r="U27" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="W27" s="81"/>
-      <c r="X27" s="81"/>
+      <c r="W27" s="89"/>
+      <c r="X27" s="89"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
@@ -3584,8 +3578,8 @@
       <c r="U28" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="W28" s="81"/>
-      <c r="X28" s="81"/>
+      <c r="W28" s="89"/>
+      <c r="X28" s="89"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
@@ -3605,7 +3599,7 @@
       </c>
       <c r="F29" s="26"/>
       <c r="G29" s="27" t="s">
-        <v>218</v>
+        <v>260</v>
       </c>
       <c r="H29" s="13">
         <v>27</v>
@@ -3645,8 +3639,8 @@
       <c r="U29" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="W29" s="81"/>
-      <c r="X29" s="81"/>
+      <c r="W29" s="89"/>
+      <c r="X29" s="89"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
@@ -3664,7 +3658,7 @@
       <c r="E30" s="12"/>
       <c r="F30" s="26"/>
       <c r="G30" s="27" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H30" s="13">
         <v>28</v>
@@ -3704,8 +3698,8 @@
       <c r="U30" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="W30" s="81"/>
-      <c r="X30" s="81"/>
+      <c r="W30" s="89"/>
+      <c r="X30" s="89"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
@@ -3723,7 +3717,7 @@
       <c r="E31" s="12"/>
       <c r="F31" s="26"/>
       <c r="G31" s="27" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="H31" s="13">
         <v>29</v>
@@ -3763,8 +3757,8 @@
       <c r="U31" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="W31" s="81"/>
-      <c r="X31" s="81"/>
+      <c r="W31" s="89"/>
+      <c r="X31" s="89"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
@@ -3777,7 +3771,7 @@
         <v>91</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="26"/>
@@ -3822,7 +3816,7 @@
         <v>91</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="26"/>
@@ -3879,12 +3873,12 @@
         <v>91</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="26"/>
       <c r="G34" s="60" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H34" s="61">
         <v>32</v>
@@ -3893,7 +3887,7 @@
         <v>96</v>
       </c>
       <c r="J34" s="63" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="K34" s="14" t="s">
         <v>69</v>
@@ -3919,7 +3913,7 @@
         <v>165</v>
       </c>
       <c r="T34" s="47" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="U34" s="46" t="s">
         <v>167</v>
@@ -3927,7 +3921,7 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="73" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B36" s="74"/>
       <c r="C36" s="74"/>
@@ -3935,7 +3929,7 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="77" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B37" s="78"/>
       <c r="C37" s="78"/>
@@ -3943,12 +3937,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="W26:X31"/>
     <mergeCell ref="G1:G2"/>
@@ -3965,6 +3953,12 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4676,38 +4670,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="88" t="s">
+      <c r="D1" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="88" t="s">
+      <c r="E1" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="88" t="s">
+      <c r="F1" s="81" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="88" t="s">
+      <c r="H1" s="81" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
+      <c r="A2" s="82"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
       <c r="G2" s="97"/>
       <c r="H2" s="98"/>
     </row>
@@ -4814,10 +4808,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Correcciones a la escaleta
Palabras mal escritas, y se ajustan las observaciones de la última parte
del recurso 50
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion04/ESCALETA_CN_08_04_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion04/ESCALETA_CN_08_04_CO.xlsx
@@ -570,9 +570,6 @@
     <t>La reproducción de los microorganismos</t>
   </si>
   <si>
-    <t>Faltante. Se hace una imagen para la importancia de la reproiducción, en donde se indica que todos los seres vivos deben reproducirse, y que esto es importante para que la especie sobreviva, pues los individuos tarde o temprano mueren. En otra imagen se explican las estrategias reproductivas r y K, sus ventajas y desventajas, y ejemplos de cada una. Puede ser en varias pantallas.</t>
-  </si>
-  <si>
     <t>RF</t>
   </si>
   <si>
@@ -597,9 +594,6 @@
     <t>Actividad para reforzar la comprensión acerca de la importancia de la reproducción y las estrategias reproductivas</t>
   </si>
   <si>
-    <t>Faltante. Preguntas de respuesta libre acerca de la importancia d ela reproducción</t>
-  </si>
-  <si>
     <t>Recurso M101A-02</t>
   </si>
   <si>
@@ -612,9 +606,6 @@
     <t>Interactivo que enseña sobre la reproducción sexual y asexual y las variantes que tienen</t>
   </si>
   <si>
-    <t>Faltante. Una imagen trata sobre la reproducción asexual y otra sexual. Al tocar cada imagen y entrar a la presentación de diapositivas, la primera pantalla define el tipo de reproducción (uno o dos progenitores, genera clones o individuos diferentes). Las siguientes pantallas tienen las variantes: gemación, fisión binaria, gemación, esporulación, fisión (escición y fragmentación), partenogénesis, para reproducción asexual,  y en la parte de sexual se habla de fecundación interna y externa, y luego de desarrollo del embrión (oviparismo, ovoviviparismo, viviparismo)</t>
-  </si>
-  <si>
     <t>Actividad para identificar las características de los diferentes tipos de reproducción sexual</t>
   </si>
   <si>
@@ -805,6 +796,15 @@
   </si>
   <si>
     <t>Refuerza tu aprendizaje: La reproducción de los animales</t>
+  </si>
+  <si>
+    <t>Faltante. Se hace una imagen para la importancia de la reproducción, en donde se indica que todos los seres vivos deben reproducirse, y que esto es importante para que la especie sobreviva, pues los individuos tarde o temprano mueren. En otra imagen se explican las estrategias reproductivas r y K, sus ventajas y desventajas, y ejemplos de cada una. Puede ser en varias pantallas.</t>
+  </si>
+  <si>
+    <t>Faltante. Preguntas de respuesta libre acerca de la importancia de la reproducción</t>
+  </si>
+  <si>
+    <t>Faltante. Una imagen trata sobre la reproducción asexual y otra sexual. Al tocar cada imagen y entrar a la presentación de diapositivas, la primera pantalla define el tipo de reproducción (uno o dos progenitores, genera clones o individuos diferentes). Las siguientes pantallas tienen las variantes: gemación, fisión binaria, gemación, esporulación, fisión (escición y fragmentación), partenogénesis, para reproducción asexual,  y en la parte de sexual se habla de divisiones según los gametos: isogamia y anisogamia (incluyendo la oogamia).</t>
   </si>
 </sst>
 </file>
@@ -1414,56 +1414,56 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1747,7 +1747,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1757,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,103 +1788,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="C1" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="83" t="s">
+      <c r="E1" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="90" t="s">
+      <c r="F1" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="79" t="s">
+      <c r="G1" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="81" t="s">
+      <c r="H1" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="85" t="s">
+      <c r="I1" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="81" t="s">
+      <c r="J1" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="94" t="s">
+      <c r="K1" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="81" t="s">
+      <c r="L1" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="92" t="s">
+      <c r="M1" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="93"/>
-      <c r="O1" s="85" t="s">
+      <c r="N1" s="87"/>
+      <c r="O1" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="81" t="s">
+      <c r="P1" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="79" t="s">
+      <c r="Q1" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="81" t="s">
+      <c r="R1" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="90" t="s">
+      <c r="S1" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="81" t="s">
+      <c r="T1" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="90" t="s">
+      <c r="U1" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="87" t="s">
-        <v>241</v>
-      </c>
-      <c r="X1" s="87"/>
+      <c r="W1" s="79" t="s">
+        <v>238</v>
+      </c>
+      <c r="X1" s="79"/>
     </row>
     <row r="2" spans="1:24" s="7" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="80"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="82"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="89"/>
       <c r="M2" s="23" t="s">
         <v>87</v>
       </c>
       <c r="N2" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="86"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="91"/>
-      <c r="T2" s="82"/>
-      <c r="U2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="89"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="89"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="89"/>
+      <c r="U2" s="85"/>
       <c r="W2" s="56" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="X2" s="57" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1914,7 +1914,7 @@
         <v>94</v>
       </c>
       <c r="J3" s="63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>69</v>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="N3" s="30"/>
       <c r="O3" s="42" t="s">
-        <v>182</v>
+        <v>258</v>
       </c>
       <c r="P3" s="48" t="s">
         <v>19</v>
@@ -1936,16 +1936,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="49" t="s">
+        <v>182</v>
+      </c>
+      <c r="S3" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="S3" s="49" t="s">
+      <c r="T3" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="T3" s="53" t="s">
+      <c r="U3" s="49" t="s">
         <v>185</v>
-      </c>
-      <c r="U3" s="49" t="s">
-        <v>186</v>
       </c>
       <c r="W3" s="58">
         <v>1</v>
@@ -1972,7 +1972,7 @@
       </c>
       <c r="F4" s="26"/>
       <c r="G4" s="60" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H4" s="61">
         <v>2</v>
@@ -1981,7 +1981,7 @@
         <v>96</v>
       </c>
       <c r="J4" s="63" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>69</v>
@@ -1994,7 +1994,7 @@
         <v>24</v>
       </c>
       <c r="O4" s="42" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="P4" s="48" t="s">
         <v>19</v>
@@ -2018,7 +2018,7 @@
         <v>2</v>
       </c>
       <c r="X4" s="72" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="F5" s="26"/>
       <c r="G5" s="60" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H5" s="61">
         <v>3</v>
@@ -2048,7 +2048,7 @@
         <v>96</v>
       </c>
       <c r="J5" s="65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>69</v>
@@ -2061,7 +2061,7 @@
         <v>62</v>
       </c>
       <c r="O5" s="42" t="s">
-        <v>191</v>
+        <v>259</v>
       </c>
       <c r="P5" s="48" t="s">
         <v>20</v>
@@ -2085,7 +2085,7 @@
         <v>3</v>
       </c>
       <c r="X5" s="72" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2106,7 +2106,7 @@
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="27" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H6" s="13">
         <v>4</v>
@@ -2115,7 +2115,7 @@
         <v>96</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>69</v>
@@ -2141,7 +2141,7 @@
         <v>165</v>
       </c>
       <c r="T6" s="47" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="U6" s="46" t="s">
         <v>167</v>
@@ -2150,7 +2150,7 @@
         <v>4</v>
       </c>
       <c r="X6" s="72" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2178,7 +2178,7 @@
         <v>94</v>
       </c>
       <c r="J7" s="63" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>69</v>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="N7" s="30"/>
       <c r="O7" s="42" t="s">
-        <v>196</v>
+        <v>260</v>
       </c>
       <c r="P7" s="48" t="s">
         <v>19</v>
@@ -2200,22 +2200,22 @@
         <v>6</v>
       </c>
       <c r="R7" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="S7" s="50" t="s">
         <v>183</v>
       </c>
-      <c r="S7" s="50" t="s">
-        <v>184</v>
-      </c>
       <c r="T7" s="54" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="U7" s="50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="W7" s="58">
         <v>5</v>
       </c>
       <c r="X7" s="72" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -2282,7 +2282,7 @@
         <v>6</v>
       </c>
       <c r="X8" s="72" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:24" s="43" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2302,7 +2302,7 @@
         <v>176</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G9" s="66" t="s">
         <v>174</v>
@@ -2314,7 +2314,7 @@
         <v>96</v>
       </c>
       <c r="J9" s="63" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K9" s="38" t="s">
         <v>69</v>
@@ -2327,7 +2327,7 @@
         <v>60</v>
       </c>
       <c r="O9" s="42" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="P9" s="48" t="s">
         <v>19</v>
@@ -2342,7 +2342,7 @@
         <v>165</v>
       </c>
       <c r="T9" s="47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="U9" s="46" t="s">
         <v>167</v>
@@ -2371,10 +2371,10 @@
         <v>176</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H10" s="13">
         <v>8</v>
@@ -2409,7 +2409,7 @@
         <v>165</v>
       </c>
       <c r="T10" s="47" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="U10" s="46" t="s">
         <v>167</v>
@@ -2418,7 +2418,7 @@
         <v>8</v>
       </c>
       <c r="X10" s="72" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -2439,7 +2439,7 @@
       </c>
       <c r="F11" s="36"/>
       <c r="G11" s="60" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H11" s="61">
         <v>9</v>
@@ -2448,7 +2448,7 @@
         <v>96</v>
       </c>
       <c r="J11" s="63" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="K11" s="14" t="s">
         <v>69</v>
@@ -2461,7 +2461,7 @@
         <v>62</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="P11" s="48" t="s">
         <v>19</v>
@@ -2476,7 +2476,7 @@
         <v>165</v>
       </c>
       <c r="T11" s="47" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="U11" s="46" t="s">
         <v>167</v>
@@ -2502,7 +2502,7 @@
         <v>109</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="60" t="s">
@@ -2515,7 +2515,7 @@
         <v>94</v>
       </c>
       <c r="J12" s="63" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K12" s="14" t="s">
         <v>69</v>
@@ -2528,7 +2528,7 @@
       </c>
       <c r="N12" s="30"/>
       <c r="O12" s="42" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="P12" s="48" t="s">
         <v>19</v>
@@ -2537,16 +2537,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="S12" s="50" t="s">
         <v>183</v>
       </c>
-      <c r="S12" s="50" t="s">
-        <v>184</v>
-      </c>
       <c r="T12" s="54" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="U12" s="50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="W12" s="59">
         <v>10</v>
@@ -2569,11 +2569,11 @@
         <v>109</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="27" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H13" s="13">
         <v>11</v>
@@ -2582,7 +2582,7 @@
         <v>96</v>
       </c>
       <c r="J13" s="37" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K13" s="14" t="s">
         <v>69</v>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="F14" s="26"/>
       <c r="G14" s="60" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H14" s="61">
         <v>12</v>
@@ -2647,7 +2647,7 @@
         <v>96</v>
       </c>
       <c r="J14" s="63" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="K14" s="14" t="s">
         <v>69</v>
@@ -2660,7 +2660,7 @@
         <v>62</v>
       </c>
       <c r="O14" s="42" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="P14" s="48" t="s">
         <v>19</v>
@@ -2675,7 +2675,7 @@
         <v>165</v>
       </c>
       <c r="T14" s="47" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="U14" s="46" t="s">
         <v>167</v>
@@ -2712,7 +2712,7 @@
         <v>94</v>
       </c>
       <c r="J15" s="63" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K15" s="14" t="s">
         <v>69</v>
@@ -2725,7 +2725,7 @@
       </c>
       <c r="N15" s="30"/>
       <c r="O15" s="42" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="P15" s="48" t="s">
         <v>19</v>
@@ -2734,22 +2734,22 @@
         <v>6</v>
       </c>
       <c r="R15" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="S15" s="50" t="s">
         <v>183</v>
       </c>
-      <c r="S15" s="50" t="s">
-        <v>184</v>
-      </c>
       <c r="T15" s="54" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="U15" s="50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="W15" s="59">
         <v>13</v>
       </c>
       <c r="X15" s="72" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -2768,7 +2768,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="26"/>
       <c r="G16" s="68" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H16" s="69">
         <v>14</v>
@@ -2777,7 +2777,7 @@
         <v>94</v>
       </c>
       <c r="J16" s="71" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K16" s="14" t="s">
         <v>70</v>
@@ -2788,7 +2788,7 @@
       <c r="M16" s="31"/>
       <c r="N16" s="30"/>
       <c r="O16" s="42" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P16" s="48" t="s">
         <v>19</v>
@@ -2831,7 +2831,7 @@
       <c r="E17" s="12"/>
       <c r="F17" s="26"/>
       <c r="G17" s="27" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H17" s="13">
         <v>15</v>
@@ -2875,7 +2875,7 @@
         <v>15</v>
       </c>
       <c r="X17" s="72" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="F18" s="26"/>
       <c r="G18" s="60" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H18" s="61">
         <v>16</v>
@@ -2905,7 +2905,7 @@
         <v>96</v>
       </c>
       <c r="J18" s="63" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="K18" s="14" t="s">
         <v>69</v>
@@ -2918,7 +2918,7 @@
         <v>62</v>
       </c>
       <c r="O18" s="42" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="P18" s="48" t="s">
         <v>19</v>
@@ -2933,7 +2933,7 @@
         <v>165</v>
       </c>
       <c r="T18" s="47" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="U18" s="46" t="s">
         <v>167</v>
@@ -2970,7 +2970,7 @@
         <v>94</v>
       </c>
       <c r="J19" s="63" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="K19" s="14" t="s">
         <v>69</v>
@@ -2983,7 +2983,7 @@
       </c>
       <c r="N19" s="30"/>
       <c r="O19" s="42" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="P19" s="48" t="s">
         <v>19</v>
@@ -2992,16 +2992,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="S19" s="50" t="s">
         <v>183</v>
       </c>
-      <c r="S19" s="50" t="s">
-        <v>184</v>
-      </c>
       <c r="T19" s="54" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="U19" s="50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="W19" s="59">
         <v>17</v>
@@ -3024,11 +3024,11 @@
         <v>115</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F20" s="26"/>
       <c r="G20" s="27" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H20" s="13">
         <v>18</v>
@@ -3158,7 +3158,7 @@
       </c>
       <c r="F22" s="26"/>
       <c r="G22" s="75" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H22" s="69">
         <v>20</v>
@@ -3167,7 +3167,7 @@
         <v>94</v>
       </c>
       <c r="J22" s="76" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K22" s="14" t="s">
         <v>70</v>
@@ -3178,7 +3178,7 @@
       <c r="M22" s="31"/>
       <c r="N22" s="30"/>
       <c r="O22" s="42" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="P22" s="48" t="s">
         <v>19</v>
@@ -3202,7 +3202,7 @@
         <v>20</v>
       </c>
       <c r="X22" s="72" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="F24" s="26"/>
       <c r="G24" s="27" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H24" s="13">
         <v>22</v>
@@ -3353,7 +3353,7 @@
       </c>
       <c r="F25" s="26"/>
       <c r="G25" s="60" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H25" s="61">
         <v>23</v>
@@ -3362,7 +3362,7 @@
         <v>96</v>
       </c>
       <c r="J25" s="63" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="K25" s="14" t="s">
         <v>69</v>
@@ -3375,7 +3375,7 @@
         <v>62</v>
       </c>
       <c r="O25" s="42" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="P25" s="48" t="s">
         <v>19</v>
@@ -3390,7 +3390,7 @@
         <v>165</v>
       </c>
       <c r="T25" s="47" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="U25" s="46" t="s">
         <v>167</v>
@@ -3454,10 +3454,10 @@
       <c r="U26" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="W26" s="88" t="s">
-        <v>253</v>
-      </c>
-      <c r="X26" s="89"/>
+      <c r="W26" s="80" t="s">
+        <v>250</v>
+      </c>
+      <c r="X26" s="81"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
@@ -3517,8 +3517,8 @@
       <c r="U27" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="W27" s="89"/>
-      <c r="X27" s="89"/>
+      <c r="W27" s="81"/>
+      <c r="X27" s="81"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
@@ -3578,8 +3578,8 @@
       <c r="U28" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="W28" s="89"/>
-      <c r="X28" s="89"/>
+      <c r="W28" s="81"/>
+      <c r="X28" s="81"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
@@ -3599,7 +3599,7 @@
       </c>
       <c r="F29" s="26"/>
       <c r="G29" s="27" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H29" s="13">
         <v>27</v>
@@ -3639,8 +3639,8 @@
       <c r="U29" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="W29" s="89"/>
-      <c r="X29" s="89"/>
+      <c r="W29" s="81"/>
+      <c r="X29" s="81"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
@@ -3658,7 +3658,7 @@
       <c r="E30" s="12"/>
       <c r="F30" s="26"/>
       <c r="G30" s="27" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H30" s="13">
         <v>28</v>
@@ -3698,8 +3698,8 @@
       <c r="U30" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="W30" s="89"/>
-      <c r="X30" s="89"/>
+      <c r="W30" s="81"/>
+      <c r="X30" s="81"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
@@ -3717,7 +3717,7 @@
       <c r="E31" s="12"/>
       <c r="F31" s="26"/>
       <c r="G31" s="27" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="H31" s="13">
         <v>29</v>
@@ -3757,8 +3757,8 @@
       <c r="U31" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="W31" s="89"/>
-      <c r="X31" s="89"/>
+      <c r="W31" s="81"/>
+      <c r="X31" s="81"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
@@ -3771,7 +3771,7 @@
         <v>91</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="26"/>
@@ -3816,7 +3816,7 @@
         <v>91</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="26"/>
@@ -3873,12 +3873,12 @@
         <v>91</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="26"/>
       <c r="G34" s="60" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H34" s="61">
         <v>32</v>
@@ -3887,7 +3887,7 @@
         <v>96</v>
       </c>
       <c r="J34" s="63" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="K34" s="14" t="s">
         <v>69</v>
@@ -3913,7 +3913,7 @@
         <v>165</v>
       </c>
       <c r="T34" s="47" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="U34" s="46" t="s">
         <v>167</v>
@@ -3921,7 +3921,7 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="73" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B36" s="74"/>
       <c r="C36" s="74"/>
@@ -3929,7 +3929,7 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="77" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B37" s="78"/>
       <c r="C37" s="78"/>
@@ -3937,6 +3937,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="W26:X31"/>
     <mergeCell ref="G1:G2"/>
@@ -3953,12 +3959,6 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4670,38 +4670,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="88" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="81" t="s">
+      <c r="H1" s="88" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
       <c r="G2" s="97"/>
       <c r="H2" s="98"/>
     </row>

</xml_diff>